<commit_message>
fix sending sms bugs
</commit_message>
<xml_diff>
--- a/user-logs/data.xlsx
+++ b/user-logs/data.xlsx
@@ -5,6 +5,7 @@
   <sheets>
     <sheet name="home" sheetId="1" r:id="rId1"/>
     <sheet name="2022_2" sheetId="2" r:id="rId2"/>
+    <sheet name="2022_3" sheetId="3" r:id="rId3"/>
   </sheets>
 </workbook>
 </file>
@@ -1108,4 +1109,334 @@
     <ignoredError numberStoredAsText="1" sqref="A1:N20"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>date</v>
+      </c>
+      <c r="B1" t="str">
+        <v>time</v>
+      </c>
+      <c r="C1" t="str">
+        <v>phoneNumber</v>
+      </c>
+      <c r="D1" t="str">
+        <v>model</v>
+      </c>
+      <c r="E1" t="str">
+        <v>path</v>
+      </c>
+      <c r="F1" t="str">
+        <v>action</v>
+      </c>
+      <c r="G1" t="str">
+        <v>status</v>
+      </c>
+      <c r="H1" t="str">
+        <v>description</v>
+      </c>
+      <c r="I1" t="str">
+        <v>failureReason</v>
+      </c>
+      <c r="J1" t="str">
+        <v>userId</v>
+      </c>
+      <c r="K1" t="str">
+        <v>modelId</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Mon Mar 07 2022</v>
+      </c>
+      <c r="B2" t="str">
+        <v>07:20:39 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="C2" t="str">
+        <v>+22892942601</v>
+      </c>
+      <c r="D2" t="str">
+        <v>User</v>
+      </c>
+      <c r="E2" t="str">
+        <v>/api/auth/send-otp</v>
+      </c>
+      <c r="F2" t="str">
+        <v>request</v>
+      </c>
+      <c r="G2" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H2" t="str">
+        <v>+22892942601 request to receive otp</v>
+      </c>
+      <c r="I2" t="str">
+        <v>phoneNumber.chartAt is not a function</v>
+      </c>
+      <c r="J2" t="str">
+        <v>+22892942601 request to receive otp</v>
+      </c>
+      <c r="K2" t="str">
+        <v>phoneNumber.chartAt is not a function</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Mon Mar 07 2022</v>
+      </c>
+      <c r="B3" t="str">
+        <v>07:25:45 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="C3" t="str">
+        <v>+22892942601</v>
+      </c>
+      <c r="D3" t="str">
+        <v>User</v>
+      </c>
+      <c r="E3" t="str">
+        <v>/api/auth/send-otp</v>
+      </c>
+      <c r="F3" t="str">
+        <v>request</v>
+      </c>
+      <c r="G3" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H3" t="str">
+        <v>+22892942601 request to receive otp</v>
+      </c>
+      <c r="I3" t="str">
+        <v>phoneNumber.chartAt is not a function</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Mon Mar 07 2022</v>
+      </c>
+      <c r="B4" t="str">
+        <v>07:27:09 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="C4" t="str">
+        <v>+22892942601</v>
+      </c>
+      <c r="D4" t="str">
+        <v>User</v>
+      </c>
+      <c r="E4" t="str">
+        <v>/api/auth/send-otp</v>
+      </c>
+      <c r="F4" t="str">
+        <v>request</v>
+      </c>
+      <c r="G4" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H4" t="str">
+        <v>+22892942601 request to receive otp</v>
+      </c>
+      <c r="I4" t="str">
+        <v>phoneNumber.chartAt is not a function</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Mon Mar 07 2022</v>
+      </c>
+      <c r="B5" t="str">
+        <v>07:28:23 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="C5" t="str">
+        <v>+22892942601</v>
+      </c>
+      <c r="D5" t="str">
+        <v>User</v>
+      </c>
+      <c r="E5" t="str">
+        <v>/api/auth/send-otp</v>
+      </c>
+      <c r="F5" t="str">
+        <v>request</v>
+      </c>
+      <c r="G5" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H5" t="str">
+        <v>+22892942601 request to receive otp</v>
+      </c>
+      <c r="I5" t="str">
+        <v>Cannot read properties of undefined (reading 'apiUrl')</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Mon Mar 07 2022</v>
+      </c>
+      <c r="B6" t="str">
+        <v>07:30:00 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="C6" t="str">
+        <v>+22892942601</v>
+      </c>
+      <c r="D6" t="str">
+        <v>User</v>
+      </c>
+      <c r="E6" t="str">
+        <v>/api/auth/send-otp</v>
+      </c>
+      <c r="F6" t="str">
+        <v>request</v>
+      </c>
+      <c r="G6" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H6" t="str">
+        <v>+22892942601 request to receive otp</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Mon Mar 07 2022</v>
+      </c>
+      <c r="B7" t="str">
+        <v>07:31:44 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="C7" t="str">
+        <v>22892942601</v>
+      </c>
+      <c r="D7" t="str">
+        <v>User</v>
+      </c>
+      <c r="E7" t="str">
+        <v>/api/auth/send-otp</v>
+      </c>
+      <c r="F7" t="str">
+        <v>request</v>
+      </c>
+      <c r="G7" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H7" t="str">
+        <v>22892942601 request to receive otp</v>
+      </c>
+      <c r="I7" t="str">
+        <v>error.invalid</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Mon Mar 07 2022</v>
+      </c>
+      <c r="B8" t="str">
+        <v>07:34:17 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="C8" t="str">
+        <v>22892942601</v>
+      </c>
+      <c r="D8" t="str">
+        <v>User</v>
+      </c>
+      <c r="E8" t="str">
+        <v>/api/auth/send-otp</v>
+      </c>
+      <c r="F8" t="str">
+        <v>request</v>
+      </c>
+      <c r="G8" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H8" t="str">
+        <v>22892942601 request to receive otp</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>Mon Mar 07 2022</v>
+      </c>
+      <c r="B9" t="str">
+        <v>07:38:55 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="C9" t="str">
+        <v>22892942601</v>
+      </c>
+      <c r="D9" t="str">
+        <v>User</v>
+      </c>
+      <c r="E9" t="str">
+        <v>/api/auth/send-otp</v>
+      </c>
+      <c r="F9" t="str">
+        <v>request</v>
+      </c>
+      <c r="G9" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H9" t="str">
+        <v>22892942601 request to receive otp</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Mon Mar 07 2022</v>
+      </c>
+      <c r="B10" t="str">
+        <v>07:41:48 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="C10" t="str">
+        <v>22892942601</v>
+      </c>
+      <c r="D10" t="str">
+        <v>User</v>
+      </c>
+      <c r="E10" t="str">
+        <v>/api/auth/send-otp</v>
+      </c>
+      <c r="F10" t="str">
+        <v>request</v>
+      </c>
+      <c r="G10" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H10" t="str">
+        <v>22892942601 request to receive otp</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>Mon Mar 07 2022</v>
+      </c>
+      <c r="B11" t="str">
+        <v>07:46:33 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="C11" t="str">
+        <v>22892942601</v>
+      </c>
+      <c r="D11" t="str">
+        <v>User</v>
+      </c>
+      <c r="E11" t="str">
+        <v>/api/auth/send-otp</v>
+      </c>
+      <c r="F11" t="str">
+        <v>request</v>
+      </c>
+      <c r="G11" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H11" t="str">
+        <v>22892942601 request to receive otp</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:K11"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix invalid token issue
</commit_message>
<xml_diff>
--- a/user-logs/data.xlsx
+++ b/user-logs/data.xlsx
@@ -1113,7 +1113,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:N43"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1152,6 +1152,15 @@
       <c r="K1" t="str">
         <v>modelId</v>
       </c>
+      <c r="L1" t="str">
+        <v>email</v>
+      </c>
+      <c r="M1" t="str">
+        <v>lastName</v>
+      </c>
+      <c r="N1" t="str">
+        <v>firstName</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -1434,9 +1443,1030 @@
         <v>22892942601 request to receive otp</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>Mon Mar 07 2022</v>
+      </c>
+      <c r="B12" t="str">
+        <v>07:54:48 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="D12" t="str">
+        <v>User</v>
+      </c>
+      <c r="E12" t="str">
+        <v>/api/auth/verify-email</v>
+      </c>
+      <c r="F12" t="str">
+        <v>login</v>
+      </c>
+      <c r="G12" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H12" t="str">
+        <v>k0d3.s0n1k@gmail.com  login</v>
+      </c>
+      <c r="I12" t="str">
+        <v>error.invalid</v>
+      </c>
+      <c r="L12" t="str">
+        <v>k0d3.s0n1k@gmail.com</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>Mon Mar 07 2022</v>
+      </c>
+      <c r="B13" t="str">
+        <v>07:56:13 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="D13" t="str">
+        <v>User</v>
+      </c>
+      <c r="E13" t="str">
+        <v>/api/auth/verify-email</v>
+      </c>
+      <c r="F13" t="str">
+        <v>login</v>
+      </c>
+      <c r="G13" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H13" t="str">
+        <v>k0d3.s0n1k@gmail.com  login</v>
+      </c>
+      <c r="I13" t="str">
+        <v>error.invalid</v>
+      </c>
+      <c r="L13" t="str">
+        <v>k0d3.s0n1k@gmail.com</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>Mon Mar 07 2022</v>
+      </c>
+      <c r="B14" t="str">
+        <v>07:57:30 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="D14" t="str">
+        <v>User</v>
+      </c>
+      <c r="E14" t="str">
+        <v>/api/auth/verify-email</v>
+      </c>
+      <c r="F14" t="str">
+        <v>login</v>
+      </c>
+      <c r="G14" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H14" t="str">
+        <v>k0d3.s0n1k@gmail.com  login</v>
+      </c>
+      <c r="I14" t="str">
+        <v>error.invalid</v>
+      </c>
+      <c r="L14" t="str">
+        <v>k0d3.s0n1k@gmail.com</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>Mon Mar 07 2022</v>
+      </c>
+      <c r="B15" t="str">
+        <v>07:58:06 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="D15" t="str">
+        <v>User</v>
+      </c>
+      <c r="E15" t="str">
+        <v>/api/auth/login</v>
+      </c>
+      <c r="F15" t="str">
+        <v>login</v>
+      </c>
+      <c r="G15" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H15" t="str">
+        <v>k0d3.s0n1k@gmail.com  login</v>
+      </c>
+      <c r="I15" t="str">
+        <v>error.invalid</v>
+      </c>
+      <c r="L15" t="str">
+        <v>k0d3.s0n1k@gmail.com</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>Mon Mar 07 2022</v>
+      </c>
+      <c r="B16" t="str">
+        <v>08:01:12 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="C16" t="str">
+        <v>22892942601</v>
+      </c>
+      <c r="D16" t="str">
+        <v>User</v>
+      </c>
+      <c r="E16" t="str">
+        <v>/api/auth/verify-otp</v>
+      </c>
+      <c r="F16" t="str">
+        <v>request</v>
+      </c>
+      <c r="G16" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H16" t="str">
+        <v>22892942601 request to receive otp</v>
+      </c>
+      <c r="I16" t="str">
+        <v>error.missing</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>Mon Mar 07 2022</v>
+      </c>
+      <c r="B17" t="str">
+        <v>08:02:08 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="C17" t="str">
+        <v>22892942601</v>
+      </c>
+      <c r="D17" t="str">
+        <v>User</v>
+      </c>
+      <c r="E17" t="str">
+        <v>/api/auth/verify-otp</v>
+      </c>
+      <c r="F17" t="str">
+        <v>request</v>
+      </c>
+      <c r="G17" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H17" t="str">
+        <v>22892942601 request to receive otp</v>
+      </c>
+      <c r="J17">
+        <v>2</v>
+      </c>
+      <c r="K17" t="str">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>Mon Mar 07 2022</v>
+      </c>
+      <c r="B18" t="str">
+        <v>08:05:54 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="D18" t="str">
+        <v>User</v>
+      </c>
+      <c r="E18" t="str">
+        <v>/api/auth/complete-infos</v>
+      </c>
+      <c r="F18" t="str">
+        <v>edit</v>
+      </c>
+      <c r="G18" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H18" t="str">
+        <v xml:space="preserve">    edit his infos</v>
+      </c>
+      <c r="J18">
+        <v>2</v>
+      </c>
+      <c r="K18" t="str">
+        <v>2</v>
+      </c>
+      <c r="M18" t="str">
+        <v/>
+      </c>
+      <c r="N18" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>Mon Mar 07 2022</v>
+      </c>
+      <c r="B19" t="str">
+        <v>08:07:45 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="D19" t="str">
+        <v>User</v>
+      </c>
+      <c r="E19" t="str">
+        <v>/api/auth/profile</v>
+      </c>
+      <c r="F19" t="str">
+        <v>read</v>
+      </c>
+      <c r="G19" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H19" t="str">
+        <v>Sonik  Kode  read his infos</v>
+      </c>
+      <c r="J19">
+        <v>2</v>
+      </c>
+      <c r="K19" t="str">
+        <v>2</v>
+      </c>
+      <c r="M19" t="str">
+        <v>Sonik</v>
+      </c>
+      <c r="N19" t="str">
+        <v>Kode</v>
+      </c>
+    </row>
+    <row r="20" xml:space="preserve">
+      <c r="A20" t="str">
+        <v>Mon Mar 07 2022</v>
+      </c>
+      <c r="B20" t="str">
+        <v>09:04:01 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="D20" t="str">
+        <v>User</v>
+      </c>
+      <c r="E20" t="str">
+        <v>/api/auth/add-email-auth</v>
+      </c>
+      <c r="F20" t="str">
+        <v>edit</v>
+      </c>
+      <c r="G20" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H20" t="str">
+        <v>Sonik  Kode  edit his infos</v>
+      </c>
+      <c r="I20" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+Invalid `prisma.user.findFirst()` invocation:
+{
+  where: {
+    id: 2,
+    deletedAt: null
+  },
+  select: {
+?   email?: true,
+?   password?: true,
+?   firstName?: true,
+    lang: true,
+    ~~~~
+?   id?: true,
+?   countryId?: true,
+?   avatar?: true,
+?   phoneNumber?: true,
+?   emailVerifiedAt?: true,
+?   phoneNumberVerifiedAt?: true,
+?   lastName?: true,
+?   birthDay?: true,
+?   status?: true,
+?   role?: true,
+?   language?: true,
+?   idCard?: true,
+?   driverLicence?: true,
+?   rating?: true,
+?   createdAt?: true,
+?   blockedAt?: true,
+?   updatedAt?: true,
+?   profileCompletedAt?: true,
+?   deletedAt?: true,
+?   deletionReport?: true,
+?   operations?: true,
+?   preferences?: true,
+?   trips?: true,
+?   travels?: true,
+?   vehicles?: true,
+?   historics?: true,
+?   sendedNotifications?: true,
+?   receivedNotifications?: true,
+?   wallets?: true,
+?   devices?: true,
+?   country?: true,
+?   _count?: true
+  }
+}
+Unknown field `lang` for select statement on model User. Available options are listed in green. Did you mean `rating`?
+</v>
+      </c>
+      <c r="J20">
+        <v>2</v>
+      </c>
+      <c r="K20" t="str">
+        <v>2</v>
+      </c>
+      <c r="M20" t="str">
+        <v>Sonik</v>
+      </c>
+      <c r="N20" t="str">
+        <v>Kode</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>Mon Mar 07 2022</v>
+      </c>
+      <c r="B21" t="str">
+        <v>09:09:07 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="D21" t="str">
+        <v>User</v>
+      </c>
+      <c r="E21" t="str">
+        <v>/api/auth/add-email-auth</v>
+      </c>
+      <c r="F21" t="str">
+        <v>edit</v>
+      </c>
+      <c r="G21" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H21" t="str">
+        <v>Sonik  Kode  edit his infos</v>
+      </c>
+      <c r="J21">
+        <v>2</v>
+      </c>
+      <c r="K21" t="str">
+        <v>2</v>
+      </c>
+      <c r="M21" t="str">
+        <v>Sonik</v>
+      </c>
+      <c r="N21" t="str">
+        <v>Kode</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>Mon Mar 07 2022</v>
+      </c>
+      <c r="B22" t="str">
+        <v>09:12:57 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="D22" t="str">
+        <v>User</v>
+      </c>
+      <c r="E22" t="str">
+        <v>/api/auth/verify-email</v>
+      </c>
+      <c r="F22" t="str">
+        <v>login</v>
+      </c>
+      <c r="G22" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H22" t="str">
+        <v>k0d3.s0n1k@gmail.com  login</v>
+      </c>
+      <c r="I22" t="str">
+        <v>error.unauthorized</v>
+      </c>
+      <c r="L22" t="str">
+        <v>k0d3.s0n1k@gmail.com</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>Mon Mar 07 2022</v>
+      </c>
+      <c r="B23" t="str">
+        <v>09:28:45 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="D23" t="str">
+        <v>User</v>
+      </c>
+      <c r="E23" t="str">
+        <v>/api/auth/confirm-email</v>
+      </c>
+      <c r="F23" t="str">
+        <v>activate</v>
+      </c>
+      <c r="G23" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H23" t="str">
+        <v>k0d3.s0n1k@gmail.com activate his account</v>
+      </c>
+      <c r="K23" t="str">
+        <v/>
+      </c>
+      <c r="L23" t="str">
+        <v>k0d3.s0n1k@gmail.com</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>Mon Mar 07 2022</v>
+      </c>
+      <c r="B24" t="str">
+        <v>09:34:56 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="D24" t="str">
+        <v>User</v>
+      </c>
+      <c r="E24" t="str">
+        <v>/api/auth/verify-email</v>
+      </c>
+      <c r="F24" t="str">
+        <v>login</v>
+      </c>
+      <c r="G24" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H24" t="str">
+        <v>k0d3.s0n1k@gmail.com  login</v>
+      </c>
+      <c r="L24" t="str">
+        <v>k0d3.s0n1k@gmail.com</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>Mon Mar 07 2022</v>
+      </c>
+      <c r="B25" t="str">
+        <v>09:35:47 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="D25" t="str">
+        <v>User</v>
+      </c>
+      <c r="E25" t="str">
+        <v>/api/auth/verify-otp</v>
+      </c>
+      <c r="F25" t="str">
+        <v>request</v>
+      </c>
+      <c r="G25" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H25" t="str">
+        <v>undefined request to receive otp</v>
+      </c>
+      <c r="I25" t="str">
+        <v>error.missing</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>Mon Mar 07 2022</v>
+      </c>
+      <c r="B26" t="str">
+        <v>09:37:54 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="D26" t="str">
+        <v>User</v>
+      </c>
+      <c r="E26" t="str">
+        <v>/api/auth/verify-password</v>
+      </c>
+      <c r="F26" t="str">
+        <v>login</v>
+      </c>
+      <c r="G26" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H26" t="str">
+        <v>2  login</v>
+      </c>
+      <c r="I26" t="str">
+        <v>error.invalid</v>
+      </c>
+      <c r="J26">
+        <v>2</v>
+      </c>
+      <c r="K26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>Mon Mar 07 2022</v>
+      </c>
+      <c r="B27" t="str">
+        <v>09:38:05 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="D27" t="str">
+        <v>User</v>
+      </c>
+      <c r="E27" t="str">
+        <v>/api/auth/verify-email</v>
+      </c>
+      <c r="F27" t="str">
+        <v>login</v>
+      </c>
+      <c r="G27" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H27" t="str">
+        <v>k0d3.s0n1k@gmail.com  login</v>
+      </c>
+      <c r="L27" t="str">
+        <v>k0d3.s0n1k@gmail.com</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>Mon Mar 07 2022</v>
+      </c>
+      <c r="B28" t="str">
+        <v>09:38:31 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="D28" t="str">
+        <v>User</v>
+      </c>
+      <c r="E28" t="str">
+        <v>/api/auth/verify-password</v>
+      </c>
+      <c r="F28" t="str">
+        <v>login</v>
+      </c>
+      <c r="G28" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H28" t="str">
+        <v>2  login</v>
+      </c>
+      <c r="I28" t="str">
+        <v>error.invalid</v>
+      </c>
+      <c r="J28">
+        <v>2</v>
+      </c>
+      <c r="K28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>Mon Mar 07 2022</v>
+      </c>
+      <c r="B29" t="str">
+        <v>09:38:52 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="D29" t="str">
+        <v>User</v>
+      </c>
+      <c r="E29" t="str">
+        <v>/api/auth/verify-password</v>
+      </c>
+      <c r="F29" t="str">
+        <v>login</v>
+      </c>
+      <c r="G29" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H29" t="str">
+        <v>2  login</v>
+      </c>
+      <c r="I29" t="str">
+        <v>error.invalid</v>
+      </c>
+      <c r="J29">
+        <v>2</v>
+      </c>
+      <c r="K29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>Mon Mar 07 2022</v>
+      </c>
+      <c r="B30" t="str">
+        <v>09:40:34 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="D30" t="str">
+        <v>User</v>
+      </c>
+      <c r="E30" t="str">
+        <v>/api/auth/verify-email</v>
+      </c>
+      <c r="F30" t="str">
+        <v>login</v>
+      </c>
+      <c r="G30" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H30" t="str">
+        <v>k0d3.s0n1k@gmail.com  login</v>
+      </c>
+      <c r="L30" t="str">
+        <v>k0d3.s0n1k@gmail.com</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>Mon Mar 07 2022</v>
+      </c>
+      <c r="B31" t="str">
+        <v>09:43:02 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="C31" t="str">
+        <v>22892942601</v>
+      </c>
+      <c r="D31" t="str">
+        <v>User</v>
+      </c>
+      <c r="E31" t="str">
+        <v>/api/auth/send-otp</v>
+      </c>
+      <c r="F31" t="str">
+        <v>request</v>
+      </c>
+      <c r="G31" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H31" t="str">
+        <v>22892942601 request to receive otp</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>Mon Mar 07 2022</v>
+      </c>
+      <c r="B32" t="str">
+        <v>09:45:09 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="D32" t="str">
+        <v>User</v>
+      </c>
+      <c r="E32" t="str">
+        <v>/api/auth/verify-password</v>
+      </c>
+      <c r="F32" t="str">
+        <v>login</v>
+      </c>
+      <c r="G32" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H32" t="str">
+        <v>2  login</v>
+      </c>
+      <c r="I32" t="str">
+        <v>error.invalid</v>
+      </c>
+      <c r="J32">
+        <v>2</v>
+      </c>
+      <c r="K32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>Mon Mar 07 2022</v>
+      </c>
+      <c r="B33" t="str">
+        <v>09:45:43 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="C33" t="str">
+        <v>22892942601</v>
+      </c>
+      <c r="D33" t="str">
+        <v>User</v>
+      </c>
+      <c r="E33" t="str">
+        <v>/api/auth/verify-otp</v>
+      </c>
+      <c r="F33" t="str">
+        <v>request</v>
+      </c>
+      <c r="G33" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H33" t="str">
+        <v>22892942601 request to receive otp</v>
+      </c>
+      <c r="I33" t="str">
+        <v>error.invalid</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>Mon Mar 07 2022</v>
+      </c>
+      <c r="B34" t="str">
+        <v>09:48:44 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="D34" t="str">
+        <v>User</v>
+      </c>
+      <c r="E34" t="str">
+        <v>/api/auth/verify-password</v>
+      </c>
+      <c r="F34" t="str">
+        <v>login</v>
+      </c>
+      <c r="G34" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H34" t="str">
+        <v>2  login</v>
+      </c>
+      <c r="I34" t="str">
+        <v>error.invalid</v>
+      </c>
+      <c r="J34">
+        <v>2</v>
+      </c>
+      <c r="K34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>Mon Mar 07 2022</v>
+      </c>
+      <c r="B35" t="str">
+        <v>09:48:51 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="D35" t="str">
+        <v>User</v>
+      </c>
+      <c r="E35" t="str">
+        <v>/api/auth/verify-email</v>
+      </c>
+      <c r="F35" t="str">
+        <v>login</v>
+      </c>
+      <c r="G35" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H35" t="str">
+        <v>k0d3.s0n1k@gmail.com  login</v>
+      </c>
+      <c r="L35" t="str">
+        <v>k0d3.s0n1k@gmail.com</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>Mon Mar 07 2022</v>
+      </c>
+      <c r="B36" t="str">
+        <v>09:49:17 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="D36" t="str">
+        <v>User</v>
+      </c>
+      <c r="E36" t="str">
+        <v>/api/auth/verify-password</v>
+      </c>
+      <c r="F36" t="str">
+        <v>login</v>
+      </c>
+      <c r="G36" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H36" t="str">
+        <v>2  login</v>
+      </c>
+      <c r="I36" t="str">
+        <v>error.invalid</v>
+      </c>
+      <c r="J36">
+        <v>2</v>
+      </c>
+      <c r="K36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" xml:space="preserve">
+      <c r="A37" t="str">
+        <v>Mon Mar 07 2022</v>
+      </c>
+      <c r="B37" t="str">
+        <v>19:19:47 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="D37" t="str">
+        <v>User</v>
+      </c>
+      <c r="E37" t="str">
+        <v>/api/auth/verify-email</v>
+      </c>
+      <c r="F37" t="str">
+        <v>login</v>
+      </c>
+      <c r="G37" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H37" t="str">
+        <v>k0d3.s0n1k@gmail.com  login</v>
+      </c>
+      <c r="I37" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+Invalid `prisma.user.findFirst()` invocation:
+  Can't reach database server at `ec2-54-216-17-9.eu-west-1.compute.amazonaws.com`:`5432`
+Please make sure your database server is running at `ec2-54-216-17-9.eu-west-1.compute.amazonaws.com`:`5432`.</v>
+      </c>
+      <c r="L37" t="str">
+        <v>k0d3.s0n1k@gmail.com</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>Mon Mar 07 2022</v>
+      </c>
+      <c r="B38" t="str">
+        <v>19:22:31 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="D38" t="str">
+        <v>User</v>
+      </c>
+      <c r="E38" t="str">
+        <v>/api/auth/verify-password</v>
+      </c>
+      <c r="F38" t="str">
+        <v>login</v>
+      </c>
+      <c r="G38" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H38" t="str">
+        <v>2  login</v>
+      </c>
+      <c r="I38" t="str">
+        <v>error.invalid</v>
+      </c>
+      <c r="J38">
+        <v>2</v>
+      </c>
+      <c r="K38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" xml:space="preserve">
+      <c r="A39" t="str">
+        <v>Mon Mar 07 2022</v>
+      </c>
+      <c r="B39" t="str">
+        <v>19:22:36 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="D39" t="str">
+        <v>User</v>
+      </c>
+      <c r="E39" t="str">
+        <v>/api/auth/verify-email</v>
+      </c>
+      <c r="F39" t="str">
+        <v>login</v>
+      </c>
+      <c r="G39" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H39" t="str">
+        <v>k0d3.s0n1k@gmail.com  login</v>
+      </c>
+      <c r="I39" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+Invalid `prisma.user.findFirst()` invocation:
+  Can't reach database server at `ec2-54-216-17-9.eu-west-1.compute.amazonaws.com`:`5432`
+Please make sure your database server is running at `ec2-54-216-17-9.eu-west-1.compute.amazonaws.com`:`5432`.</v>
+      </c>
+      <c r="L39" t="str">
+        <v>k0d3.s0n1k@gmail.com</v>
+      </c>
+    </row>
+    <row r="40" xml:space="preserve">
+      <c r="A40" t="str">
+        <v>Mon Mar 07 2022</v>
+      </c>
+      <c r="B40" t="str">
+        <v>22:51:37 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="D40" t="str">
+        <v>User</v>
+      </c>
+      <c r="E40" t="str">
+        <v>/api/auth/verify-email</v>
+      </c>
+      <c r="F40" t="str">
+        <v>login</v>
+      </c>
+      <c r="G40" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H40" t="str">
+        <v>k0d3.s0n1k@gmail.com  login</v>
+      </c>
+      <c r="I40" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+Invalid `prisma.user.findFirst()` invocation:
+  Can't reach database server at `ec2-54-216-17-9.eu-west-1.compute.amazonaws.com`:`5432`
+Please make sure your database server is running at `ec2-54-216-17-9.eu-west-1.compute.amazonaws.com`:`5432`.</v>
+      </c>
+      <c r="L40" t="str">
+        <v>k0d3.s0n1k@gmail.com</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>Mon Mar 07 2022</v>
+      </c>
+      <c r="B41" t="str">
+        <v>22:54:10 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="D41" t="str">
+        <v>User</v>
+      </c>
+      <c r="E41" t="str">
+        <v>/api/auth/verify-email</v>
+      </c>
+      <c r="F41" t="str">
+        <v>login</v>
+      </c>
+      <c r="G41" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H41" t="str">
+        <v>k0d3.s0n1k@gmail.com  login</v>
+      </c>
+      <c r="L41" t="str">
+        <v>k0d3.s0n1k@gmail.com</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>Mon Mar 07 2022</v>
+      </c>
+      <c r="B42" t="str">
+        <v>22:56:48 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="D42" t="str">
+        <v>User</v>
+      </c>
+      <c r="E42" t="str">
+        <v>/api/auth/verify-password</v>
+      </c>
+      <c r="F42" t="str">
+        <v>login</v>
+      </c>
+      <c r="G42" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H42" t="str">
+        <v>2  login</v>
+      </c>
+      <c r="I42" t="str">
+        <v>error.invalid</v>
+      </c>
+      <c r="J42">
+        <v>2</v>
+      </c>
+      <c r="K42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>Mon Mar 07 2022</v>
+      </c>
+      <c r="B43" t="str">
+        <v>22:58:40 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="D43" t="str">
+        <v>User</v>
+      </c>
+      <c r="E43" t="str">
+        <v>/api/auth/verify-password</v>
+      </c>
+      <c r="F43" t="str">
+        <v>login</v>
+      </c>
+      <c r="G43" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H43" t="str">
+        <v>2  login</v>
+      </c>
+      <c r="I43" t="str">
+        <v>error.invalid</v>
+      </c>
+      <c r="J43">
+        <v>2</v>
+      </c>
+      <c r="K43">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N43"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add signup for phonenumber
</commit_message>
<xml_diff>
--- a/user-logs/data.xlsx
+++ b/user-logs/data.xlsx
@@ -2596,7 +2596,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M70"/>
+  <dimension ref="A1:M78"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -5922,9 +5922,235 @@
         <v>TAGBA</v>
       </c>
     </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>Mon Apr 25 2022</v>
+      </c>
+      <c r="B71" t="str">
+        <v>11:42:18 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="C71" t="str">
+        <v>22892942600</v>
+      </c>
+      <c r="D71" t="str">
+        <v>User</v>
+      </c>
+      <c r="E71" t="str">
+        <v>/api/auth/send-otp</v>
+      </c>
+      <c r="F71" t="str">
+        <v>request</v>
+      </c>
+      <c r="G71" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H71" t="str">
+        <v>22892942600 request to receive otp</v>
+      </c>
+      <c r="M71" t="str">
+        <v>Cannot read properties of undefined (reading 'findFirst')</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>Mon Apr 25 2022</v>
+      </c>
+      <c r="B72" t="str">
+        <v>11:43:20 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="C72" t="str">
+        <v>22892942600</v>
+      </c>
+      <c r="D72" t="str">
+        <v>User</v>
+      </c>
+      <c r="E72" t="str">
+        <v>/api/auth/send-otp</v>
+      </c>
+      <c r="F72" t="str">
+        <v>request</v>
+      </c>
+      <c r="G72" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H72" t="str">
+        <v>22892942600 request to receive otp</v>
+      </c>
+      <c r="M72" t="str">
+        <v>error.invalid</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>Mon Apr 25 2022</v>
+      </c>
+      <c r="B73" t="str">
+        <v>11:43:42 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="C73" t="str">
+        <v>22892942601</v>
+      </c>
+      <c r="D73" t="str">
+        <v>User</v>
+      </c>
+      <c r="E73" t="str">
+        <v>/api/auth/send-otp</v>
+      </c>
+      <c r="F73" t="str">
+        <v>request</v>
+      </c>
+      <c r="G73" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H73" t="str">
+        <v>22892942601 request to receive otp</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>Mon Apr 25 2022</v>
+      </c>
+      <c r="B74" t="str">
+        <v>11:43:57 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="C74" t="str">
+        <v>22892942600</v>
+      </c>
+      <c r="D74" t="str">
+        <v>User</v>
+      </c>
+      <c r="E74" t="str">
+        <v>/api/auth/send-otp</v>
+      </c>
+      <c r="F74" t="str">
+        <v>request</v>
+      </c>
+      <c r="G74" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H74" t="str">
+        <v>22892942600 request to receive otp</v>
+      </c>
+      <c r="M74" t="str">
+        <v>error.invalid</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>Mon Apr 25 2022</v>
+      </c>
+      <c r="B75" t="str">
+        <v>11:44:05 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="C75" t="str">
+        <v>22892942600</v>
+      </c>
+      <c r="D75" t="str">
+        <v>User</v>
+      </c>
+      <c r="E75" t="str">
+        <v>/api/auth/send-otp</v>
+      </c>
+      <c r="F75" t="str">
+        <v>request</v>
+      </c>
+      <c r="G75" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H75" t="str">
+        <v>22892942600 request to receive otp</v>
+      </c>
+      <c r="M75" t="str">
+        <v>error.invalid</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>Mon Apr 25 2022</v>
+      </c>
+      <c r="B76" t="str">
+        <v>11:44:12 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="C76" t="str">
+        <v>22892942600</v>
+      </c>
+      <c r="D76" t="str">
+        <v>User</v>
+      </c>
+      <c r="E76" t="str">
+        <v>/api/auth/send-otp</v>
+      </c>
+      <c r="F76" t="str">
+        <v>request</v>
+      </c>
+      <c r="G76" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H76" t="str">
+        <v>22892942600 request to receive otp</v>
+      </c>
+      <c r="M76" t="str">
+        <v>error.invalid</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>Mon Apr 25 2022</v>
+      </c>
+      <c r="B77" t="str">
+        <v>11:44:43 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="C77" t="str">
+        <v>22892942600</v>
+      </c>
+      <c r="D77" t="str">
+        <v>User</v>
+      </c>
+      <c r="E77" t="str">
+        <v>/api/auth/send-otp</v>
+      </c>
+      <c r="F77" t="str">
+        <v>request</v>
+      </c>
+      <c r="G77" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H77" t="str">
+        <v>22892942600 request to receive otp</v>
+      </c>
+      <c r="M77" t="str">
+        <v>error.invalid</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v>Mon Apr 25 2022</v>
+      </c>
+      <c r="B78" t="str">
+        <v>11:47:17 GMT+0000 (Greenwich Mean Time)</v>
+      </c>
+      <c r="C78" t="str">
+        <v>22892942600</v>
+      </c>
+      <c r="D78" t="str">
+        <v>User</v>
+      </c>
+      <c r="E78" t="str">
+        <v>/api/auth/send-otp</v>
+      </c>
+      <c r="F78" t="str">
+        <v>request</v>
+      </c>
+      <c r="G78" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H78" t="str">
+        <v>22892942600 request to receive otp</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M70"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M78"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add docker to project
</commit_message>
<xml_diff>
--- a/user-logs/data.xlsx
+++ b/user-logs/data.xlsx
@@ -8,6 +8,7 @@
     <sheet name="2022_3" sheetId="3" r:id="rId3"/>
     <sheet name="2022_4" sheetId="4" r:id="rId4"/>
     <sheet name="2022_5" sheetId="5" r:id="rId5"/>
+    <sheet name="2022_7" sheetId="6" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
@@ -6673,4 +6674,332 @@
     <ignoredError numberStoredAsText="1" sqref="A1:K17"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>date</v>
+      </c>
+      <c r="B1" t="str">
+        <v>time</v>
+      </c>
+      <c r="C1" t="str">
+        <v>phoneNumber</v>
+      </c>
+      <c r="D1" t="str">
+        <v>model</v>
+      </c>
+      <c r="E1" t="str">
+        <v>path</v>
+      </c>
+      <c r="F1" t="str">
+        <v>action</v>
+      </c>
+      <c r="G1" t="str">
+        <v>status</v>
+      </c>
+      <c r="H1" t="str">
+        <v>description</v>
+      </c>
+      <c r="I1" t="str">
+        <v>failureReason</v>
+      </c>
+      <c r="J1" t="str">
+        <v>userId</v>
+      </c>
+      <c r="K1" t="str">
+        <v>modelId</v>
+      </c>
+      <c r="L1" t="str">
+        <v>lastName</v>
+      </c>
+      <c r="M1" t="str">
+        <v>firstName</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Sat Jul 09 2022</v>
+      </c>
+      <c r="B2" t="str">
+        <v>16:12:36 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="C2" t="str">
+        <v>+22892942601</v>
+      </c>
+      <c r="D2" t="str">
+        <v>User</v>
+      </c>
+      <c r="E2" t="str">
+        <v>/api/auth/send-otp</v>
+      </c>
+      <c r="F2" t="str">
+        <v>request</v>
+      </c>
+      <c r="G2" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H2" t="str">
+        <v>+22892942601 request to receive otp</v>
+      </c>
+      <c r="I2" t="str">
+        <v>error.invalid</v>
+      </c>
+      <c r="J2" t="str">
+        <v>+22892942601 request to receive otp</v>
+      </c>
+      <c r="K2" t="str">
+        <v>error.invalid</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Sat Jul 09 2022</v>
+      </c>
+      <c r="B3" t="str">
+        <v>16:13:00 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="C3" t="str">
+        <v>22892942601</v>
+      </c>
+      <c r="D3" t="str">
+        <v>User</v>
+      </c>
+      <c r="E3" t="str">
+        <v>/api/auth/send-otp</v>
+      </c>
+      <c r="F3" t="str">
+        <v>request</v>
+      </c>
+      <c r="G3" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H3" t="str">
+        <v>22892942601 request to receive otp</v>
+      </c>
+      <c r="I3" t="str">
+        <v>error.userNotFound</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Sat Jul 09 2022</v>
+      </c>
+      <c r="B4" t="str">
+        <v>16:13:52 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="C4" t="str">
+        <v>22892942601</v>
+      </c>
+      <c r="D4" t="str">
+        <v>User</v>
+      </c>
+      <c r="E4" t="str">
+        <v>/api/auth/send-otp</v>
+      </c>
+      <c r="F4" t="str">
+        <v>request</v>
+      </c>
+      <c r="G4" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H4" t="str">
+        <v>22892942601 request to receive otp</v>
+      </c>
+      <c r="I4" t="str">
+        <v>error.userNotFound</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Sat Jul 09 2022</v>
+      </c>
+      <c r="B5" t="str">
+        <v>16:17:50 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="C5" t="str">
+        <v>22892942601</v>
+      </c>
+      <c r="D5" t="str">
+        <v>User</v>
+      </c>
+      <c r="E5" t="str">
+        <v>/api/auth/send-otp</v>
+      </c>
+      <c r="F5" t="str">
+        <v>request</v>
+      </c>
+      <c r="G5" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H5" t="str">
+        <v>22892942601 request to receive otp</v>
+      </c>
+      <c r="I5" t="str">
+        <v>getaddrinfo EAI_AGAIN dashboard.smszedekaa.com</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Sat Jul 09 2022</v>
+      </c>
+      <c r="B6" t="str">
+        <v>16:27:47 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="C6" t="str">
+        <v>22892942601</v>
+      </c>
+      <c r="D6" t="str">
+        <v>User</v>
+      </c>
+      <c r="E6" t="str">
+        <v>/api/auth/send-otp</v>
+      </c>
+      <c r="F6" t="str">
+        <v>request</v>
+      </c>
+      <c r="G6" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H6" t="str">
+        <v>22892942601 request to receive otp</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Sat Jul 09 2022</v>
+      </c>
+      <c r="B7" t="str">
+        <v>16:28:54 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="C7" t="str">
+        <v>22892942601</v>
+      </c>
+      <c r="D7" t="str">
+        <v>User</v>
+      </c>
+      <c r="E7" t="str">
+        <v>/api/auth/verify-otp</v>
+      </c>
+      <c r="F7" t="str">
+        <v>request</v>
+      </c>
+      <c r="G7" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H7" t="str">
+        <v>22892942601 request to receive otp</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7" t="str">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Sat Jul 09 2022</v>
+      </c>
+      <c r="B8" t="str">
+        <v>16:29:55 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D8" t="str">
+        <v>User</v>
+      </c>
+      <c r="E8" t="str">
+        <v>/api/auth/complete-infos</v>
+      </c>
+      <c r="F8" t="str">
+        <v>edit</v>
+      </c>
+      <c r="G8" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H8" t="str">
+        <v xml:space="preserve">    edit his infos</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8" t="str">
+        <v>1</v>
+      </c>
+      <c r="L8" t="str">
+        <v/>
+      </c>
+      <c r="M8" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>Sun Jul 10 2022</v>
+      </c>
+      <c r="B9" t="str">
+        <v>01:27:53 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="C9" t="str">
+        <v>22892942601</v>
+      </c>
+      <c r="D9" t="str">
+        <v>User</v>
+      </c>
+      <c r="E9" t="str">
+        <v>/api/auth/send-otp</v>
+      </c>
+      <c r="F9" t="str">
+        <v>request</v>
+      </c>
+      <c r="G9" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H9" t="str">
+        <v>22892942601 request to receive otp</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Sun Jul 10 2022</v>
+      </c>
+      <c r="B10" t="str">
+        <v>01:28:20 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="C10" t="str">
+        <v>22892942601</v>
+      </c>
+      <c r="D10" t="str">
+        <v>User</v>
+      </c>
+      <c r="E10" t="str">
+        <v>/api/auth/verify-otp</v>
+      </c>
+      <c r="F10" t="str">
+        <v>request</v>
+      </c>
+      <c r="G10" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H10" t="str">
+        <v>22892942601 request to receive otp</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10" t="str">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:M10"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
change docker ip addresses
</commit_message>
<xml_diff>
--- a/user-logs/data.xlsx
+++ b/user-logs/data.xlsx
@@ -6678,7 +6678,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N174"/>
+  <dimension ref="A1:N177"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -12795,9 +12795,236 @@
         <v>Admin</v>
       </c>
     </row>
+    <row r="175" xml:space="preserve">
+      <c r="A175" t="str">
+        <v>Fri Jul 22 2022</v>
+      </c>
+      <c r="B175" t="str">
+        <v>12:10:38 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D175" t="str">
+        <v>Travel</v>
+      </c>
+      <c r="E175" t="str">
+        <v>/api/travel</v>
+      </c>
+      <c r="F175" t="str">
+        <v>read</v>
+      </c>
+      <c r="G175" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H175" t="str">
+        <v>John  DOE  read all travels</v>
+      </c>
+      <c r="I175" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+Invalid `this.collection.findMany()` invocation in
+/app/src/db/query.ts:18:38
+  15     orderBy
+  16 }): Promise&lt;T[]&gt; {
+  17     if(env.db.softDelete) where = { ...where, deletedAt: null }
+→ 18     return await this.collection.findMany({
+           take: 100,
+           skip: 0,
+           select: {
+         ?   id?: true,
+             title: true,
+             ~~~~~
+             description: true,
+             ~~~~~~~~~~~
+         ?   createdAt?: true,
+         ?   userId?: true,
+         ?   routeId?: true,
+         ?   seats?: true,
+         ?   reamingSeats?: true,
+         ?   status?: true,
+         ?   startedAt?: true,
+         ?   finishedAt?: true,
+         ?   driverRating?: true,
+         ?   passengerRating?: true,
+         ?   operations?: true,
+         ?   user?: true,
+         ?   route?: true,
+         ?   _count?: true
+           },
+           where: {
+             deletedAt: null
+             ~~~~~~~~~
+           },
+           orderBy: undefined
+         })
+Unknown arg `deletedAt` in where.deletedAt for type TravelWhereInput. Did you mean `createdAt`? Available args:
+type TravelWhereInput {
+  AND?: TravelWhereInput | List&lt;TravelWhereInput&gt;
+  OR?: List&lt;TravelWhereInput&gt;
+  NOT?: TravelWhereInput | List&lt;TravelWhereInput&gt;
+  id?: IntFilter | Int
+  userId?: IntFilter | Int
+  routeId?: IntFilter | Int
+  seats?: IntFilter | Int
+  reamingSeats?: IntFilter | Int
+  status?: IntFilter | Int
+  createdAt?: DateTimeFilter | DateTime
+  startedAt?: DateTimeNullableFilter | DateTime | Null
+  finishedAt?: DateTimeNullableFilter | DateTime | Null
+  driverRating?: IntFilter | Int
+  passengerRating?: IntFilter | Int
+  operations?: OperationListRelationFilter
+  user?: UserRelationFilter | UserWhereInput
+  route?: RouteRelationFilter | RouteWhereInput
+}
+Unknown field `title` for select statement on model Travel. Available options are listed in green. Did you mean `id`?
+Unknown field `description` for select statement on model Travel. Available options are listed in green.
+</v>
+      </c>
+      <c r="J175">
+        <v>10</v>
+      </c>
+      <c r="K175" t="str">
+        <v>all</v>
+      </c>
+      <c r="L175" t="str">
+        <v>John</v>
+      </c>
+      <c r="M175" t="str">
+        <v>DOE</v>
+      </c>
+    </row>
+    <row r="176" xml:space="preserve">
+      <c r="A176" t="str">
+        <v>Fri Jul 22 2022</v>
+      </c>
+      <c r="B176" t="str">
+        <v>12:16:34 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D176" t="str">
+        <v>Travel</v>
+      </c>
+      <c r="E176" t="str">
+        <v>/api/travel</v>
+      </c>
+      <c r="F176" t="str">
+        <v>read</v>
+      </c>
+      <c r="G176" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H176" t="str">
+        <v>John  DOE  read all travels</v>
+      </c>
+      <c r="I176" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+Invalid `this.collection.findMany()` invocation in
+/app/src/db/query.ts:18:38
+  15     orderBy
+  16 }): Promise&lt;T[]&gt; {
+  17     if(env.db.softDelete) where = { ...where, deletedAt: null }
+→ 18     return await this.collection.findMany({
+           take: 100,
+           skip: 0,
+           select: {
+         ?   id?: true,
+             title: true,
+             ~~~~~
+             description: true,
+             ~~~~~~~~~~~
+         ?   createdAt?: true,
+         ?   userId?: true,
+         ?   routeId?: true,
+         ?   seats?: true,
+         ?   reamingSeats?: true,
+         ?   status?: true,
+         ?   startedAt?: true,
+         ?   finishedAt?: true,
+         ?   driverRating?: true,
+         ?   passengerRating?: true,
+         ?   operations?: true,
+         ?   user?: true,
+         ?   route?: true,
+         ?   _count?: true
+           },
+           where: {
+             deletedAt: null
+             ~~~~~~~~~
+           },
+           orderBy: undefined
+         })
+Unknown arg `deletedAt` in where.deletedAt for type TravelWhereInput. Did you mean `createdAt`? Available args:
+type TravelWhereInput {
+  AND?: TravelWhereInput | List&lt;TravelWhereInput&gt;
+  OR?: List&lt;TravelWhereInput&gt;
+  NOT?: TravelWhereInput | List&lt;TravelWhereInput&gt;
+  id?: IntFilter | Int
+  userId?: IntFilter | Int
+  routeId?: IntFilter | Int
+  seats?: IntFilter | Int
+  reamingSeats?: IntFilter | Int
+  status?: IntFilter | Int
+  createdAt?: DateTimeFilter | DateTime
+  startedAt?: DateTimeNullableFilter | DateTime | Null
+  finishedAt?: DateTimeNullableFilter | DateTime | Null
+  driverRating?: IntFilter | Int
+  passengerRating?: IntFilter | Int
+  operations?: OperationListRelationFilter
+  user?: UserRelationFilter | UserWhereInput
+  route?: RouteRelationFilter | RouteWhereInput
+}
+Unknown field `title` for select statement on model Travel. Available options are listed in green. Did you mean `id`?
+Unknown field `description` for select statement on model Travel. Available options are listed in green.
+</v>
+      </c>
+      <c r="J176">
+        <v>10</v>
+      </c>
+      <c r="K176" t="str">
+        <v>all</v>
+      </c>
+      <c r="L176" t="str">
+        <v>John</v>
+      </c>
+      <c r="M176" t="str">
+        <v>DOE</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="str">
+        <v>Fri Jul 22 2022</v>
+      </c>
+      <c r="B177" t="str">
+        <v>12:21:03 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D177" t="str">
+        <v>Travel</v>
+      </c>
+      <c r="E177" t="str">
+        <v>/api/travel</v>
+      </c>
+      <c r="F177" t="str">
+        <v>read</v>
+      </c>
+      <c r="G177" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H177" t="str">
+        <v>John  DOE  read all travels (undefined) from undefined to NaN</v>
+      </c>
+      <c r="J177">
+        <v>10</v>
+      </c>
+      <c r="K177" t="str">
+        <v>all</v>
+      </c>
+      <c r="L177" t="str">
+        <v>John</v>
+      </c>
+      <c r="M177" t="str">
+        <v>DOE</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N174"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N177"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
preparing to deploy on gcloud
</commit_message>
<xml_diff>
--- a/user-logs/data.xlsx
+++ b/user-logs/data.xlsx
@@ -9,6 +9,7 @@
     <sheet name="2022_4" sheetId="4" r:id="rId4"/>
     <sheet name="2022_5" sheetId="5" r:id="rId5"/>
     <sheet name="2022_7" sheetId="6" r:id="rId6"/>
+    <sheet name="2022_8" sheetId="7" r:id="rId7"/>
   </sheets>
 </workbook>
 </file>
@@ -14283,4 +14284,1258 @@
     <ignoredError numberStoredAsText="1" sqref="A1:N201"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>date</v>
+      </c>
+      <c r="B1" t="str">
+        <v>time</v>
+      </c>
+      <c r="C1" t="str">
+        <v>phoneNumber</v>
+      </c>
+      <c r="D1" t="str">
+        <v>model</v>
+      </c>
+      <c r="E1" t="str">
+        <v>path</v>
+      </c>
+      <c r="F1" t="str">
+        <v>action</v>
+      </c>
+      <c r="G1" t="str">
+        <v>status</v>
+      </c>
+      <c r="H1" t="str">
+        <v>description</v>
+      </c>
+      <c r="I1" t="str">
+        <v>failureReason</v>
+      </c>
+      <c r="J1" t="str">
+        <v>userId</v>
+      </c>
+      <c r="K1" t="str">
+        <v>modelId</v>
+      </c>
+      <c r="L1" t="str">
+        <v>lastName</v>
+      </c>
+      <c r="M1" t="str">
+        <v>firstName</v>
+      </c>
+      <c r="N1" t="str">
+        <v>email</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Sun Aug 07 2022</v>
+      </c>
+      <c r="B2" t="str">
+        <v>10:08:58 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="C2" t="str">
+        <v>22890494008</v>
+      </c>
+      <c r="D2" t="str">
+        <v>User</v>
+      </c>
+      <c r="E2" t="str">
+        <v>/api/auth/send-otp</v>
+      </c>
+      <c r="F2" t="str">
+        <v>request</v>
+      </c>
+      <c r="G2" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H2" t="str">
+        <v>22890494008 request to receive otp</v>
+      </c>
+      <c r="I2" t="str">
+        <v>error.userNotFound</v>
+      </c>
+      <c r="J2" t="str">
+        <v>22890494008 request to receive otp</v>
+      </c>
+      <c r="K2" t="str">
+        <v>error.userNotFound</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Sun Aug 07 2022</v>
+      </c>
+      <c r="B3" t="str">
+        <v>10:09:30 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="C3" t="str">
+        <v>22890494008</v>
+      </c>
+      <c r="D3" t="str">
+        <v>User</v>
+      </c>
+      <c r="E3" t="str">
+        <v>/api/auth/send-otp</v>
+      </c>
+      <c r="F3" t="str">
+        <v>request</v>
+      </c>
+      <c r="G3" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H3" t="str">
+        <v>22890494008 request to receive otp</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Sun Aug 07 2022</v>
+      </c>
+      <c r="B4" t="str">
+        <v>10:09:48 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="C4" t="str">
+        <v>22890494008</v>
+      </c>
+      <c r="D4" t="str">
+        <v>User</v>
+      </c>
+      <c r="E4" t="str">
+        <v>/api/auth/verify-otp</v>
+      </c>
+      <c r="F4" t="str">
+        <v>request</v>
+      </c>
+      <c r="G4" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H4" t="str">
+        <v>22890494008 request to receive otp</v>
+      </c>
+      <c r="J4">
+        <v>11</v>
+      </c>
+      <c r="K4" t="str">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Sun Aug 07 2022</v>
+      </c>
+      <c r="B5" t="str">
+        <v>10:10:42 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D5" t="str">
+        <v>User</v>
+      </c>
+      <c r="E5" t="str">
+        <v>/api/auth/complete-infos</v>
+      </c>
+      <c r="F5" t="str">
+        <v>edit</v>
+      </c>
+      <c r="G5" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H5" t="str">
+        <v xml:space="preserve">    edit his infos</v>
+      </c>
+      <c r="J5">
+        <v>11</v>
+      </c>
+      <c r="K5" t="str">
+        <v>11</v>
+      </c>
+      <c r="L5" t="str">
+        <v/>
+      </c>
+      <c r="M5" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Sun Aug 07 2022</v>
+      </c>
+      <c r="B6" t="str">
+        <v>10:18:50 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="C6" t="str">
+        <v>22890494008</v>
+      </c>
+      <c r="D6" t="str">
+        <v>User</v>
+      </c>
+      <c r="E6" t="str">
+        <v>/api/auth/send-otp</v>
+      </c>
+      <c r="F6" t="str">
+        <v>request</v>
+      </c>
+      <c r="G6" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H6" t="str">
+        <v>22890494008 request to receive otp</v>
+      </c>
+      <c r="I6" t="str">
+        <v>error.userNotFound</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Sun Aug 07 2022</v>
+      </c>
+      <c r="B7" t="str">
+        <v>10:19:00 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="C7" t="str">
+        <v>22890494008</v>
+      </c>
+      <c r="D7" t="str">
+        <v>User</v>
+      </c>
+      <c r="E7" t="str">
+        <v>/api/auth/send-otp</v>
+      </c>
+      <c r="F7" t="str">
+        <v>request</v>
+      </c>
+      <c r="G7" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H7" t="str">
+        <v>22890494008 request to receive otp</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Sun Aug 07 2022</v>
+      </c>
+      <c r="B8" t="str">
+        <v>10:19:40 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="C8" t="str">
+        <v>22890494008</v>
+      </c>
+      <c r="D8" t="str">
+        <v>User</v>
+      </c>
+      <c r="E8" t="str">
+        <v>/api/auth/send-otp</v>
+      </c>
+      <c r="F8" t="str">
+        <v>request</v>
+      </c>
+      <c r="G8" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H8" t="str">
+        <v>22890494008 request to receive otp</v>
+      </c>
+      <c r="I8" t="str">
+        <v>error.userNotFound</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>Sun Aug 07 2022</v>
+      </c>
+      <c r="B9" t="str">
+        <v>10:19:49 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="C9" t="str">
+        <v>22890494008</v>
+      </c>
+      <c r="D9" t="str">
+        <v>User</v>
+      </c>
+      <c r="E9" t="str">
+        <v>/api/auth/send-otp</v>
+      </c>
+      <c r="F9" t="str">
+        <v>request</v>
+      </c>
+      <c r="G9" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H9" t="str">
+        <v>22890494008 request to receive otp</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Sun Aug 07 2022</v>
+      </c>
+      <c r="B10" t="str">
+        <v>10:20:08 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="C10" t="str">
+        <v>22890494008</v>
+      </c>
+      <c r="D10" t="str">
+        <v>User</v>
+      </c>
+      <c r="E10" t="str">
+        <v>/api/auth/verify-otp</v>
+      </c>
+      <c r="F10" t="str">
+        <v>request</v>
+      </c>
+      <c r="G10" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H10" t="str">
+        <v>22890494008 request to receive otp</v>
+      </c>
+      <c r="J10">
+        <v>12</v>
+      </c>
+      <c r="K10" t="str">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>Sun Aug 07 2022</v>
+      </c>
+      <c r="B11" t="str">
+        <v>10:21:17 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D11" t="str">
+        <v>User</v>
+      </c>
+      <c r="E11" t="str">
+        <v>/api/auth/complete-infos</v>
+      </c>
+      <c r="F11" t="str">
+        <v>edit</v>
+      </c>
+      <c r="G11" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H11" t="str">
+        <v xml:space="preserve">    edit his infos</v>
+      </c>
+      <c r="J11">
+        <v>12</v>
+      </c>
+      <c r="K11" t="str">
+        <v>12</v>
+      </c>
+      <c r="L11" t="str">
+        <v/>
+      </c>
+      <c r="M11" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>Sun Aug 07 2022</v>
+      </c>
+      <c r="B12" t="str">
+        <v>11:20:21 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D12" t="str">
+        <v>User</v>
+      </c>
+      <c r="E12" t="str">
+        <v>/api/auth/login</v>
+      </c>
+      <c r="F12" t="str">
+        <v>login</v>
+      </c>
+      <c r="G12" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H12" t="str">
+        <v>test1@oreonyx.com  login</v>
+      </c>
+      <c r="I12" t="str">
+        <v>error.userNotFound</v>
+      </c>
+      <c r="N12" t="str">
+        <v>test1@oreonyx.com</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>Sun Aug 07 2022</v>
+      </c>
+      <c r="B13" t="str">
+        <v>11:22:13 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D13" t="str">
+        <v>User</v>
+      </c>
+      <c r="E13" t="str">
+        <v>/api/auth/login</v>
+      </c>
+      <c r="F13" t="str">
+        <v>login</v>
+      </c>
+      <c r="G13" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H13" t="str">
+        <v>test1@oreonyx.com  login</v>
+      </c>
+      <c r="I13" t="str">
+        <v>error.userNotFound</v>
+      </c>
+      <c r="N13" t="str">
+        <v>test1@oreonyx.com</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>Sun Aug 07 2022</v>
+      </c>
+      <c r="B14" t="str">
+        <v>11:27:22 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D14" t="str">
+        <v>User</v>
+      </c>
+      <c r="E14" t="str">
+        <v>/api/auth/login</v>
+      </c>
+      <c r="F14" t="str">
+        <v>login</v>
+      </c>
+      <c r="G14" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H14" t="str">
+        <v>test1@oreonyx.com  login</v>
+      </c>
+      <c r="I14" t="str">
+        <v>error.userNotFound</v>
+      </c>
+      <c r="N14" t="str">
+        <v>test1@oreonyx.com</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>Sun Aug 07 2022</v>
+      </c>
+      <c r="B15" t="str">
+        <v>11:27:54 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D15" t="str">
+        <v>User</v>
+      </c>
+      <c r="E15" t="str">
+        <v>/api/auth/login</v>
+      </c>
+      <c r="F15" t="str">
+        <v>login</v>
+      </c>
+      <c r="G15" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H15" t="str">
+        <v>test1@oreonyx.com  login</v>
+      </c>
+      <c r="I15" t="str">
+        <v>error.userNotFound</v>
+      </c>
+      <c r="N15" t="str">
+        <v>test1@oreonyx.com</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>Sun Aug 07 2022</v>
+      </c>
+      <c r="B16" t="str">
+        <v>11:28:37 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D16" t="str">
+        <v>User</v>
+      </c>
+      <c r="E16" t="str">
+        <v>/api/auth/login</v>
+      </c>
+      <c r="F16" t="str">
+        <v>login</v>
+      </c>
+      <c r="G16" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H16" t="str">
+        <v>test1@oreonyx.com  login</v>
+      </c>
+      <c r="I16" t="str">
+        <v>error.userNotFound</v>
+      </c>
+      <c r="N16" t="str">
+        <v>test1@oreonyx.com</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>Sun Aug 07 2022</v>
+      </c>
+      <c r="B17" t="str">
+        <v>11:28:45 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D17" t="str">
+        <v>User</v>
+      </c>
+      <c r="E17" t="str">
+        <v>/api/auth/login</v>
+      </c>
+      <c r="F17" t="str">
+        <v>login</v>
+      </c>
+      <c r="G17" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H17" t="str">
+        <v>developer@nex-softwares.com  login</v>
+      </c>
+      <c r="N17" t="str">
+        <v>developer@nex-softwares.com</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>Sun Aug 07 2022</v>
+      </c>
+      <c r="B18" t="str">
+        <v>11:46:13 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D18" t="str">
+        <v>User</v>
+      </c>
+      <c r="E18" t="str">
+        <v>/api/auth/login</v>
+      </c>
+      <c r="F18" t="str">
+        <v>login</v>
+      </c>
+      <c r="G18" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H18" t="str">
+        <v>developer@nex-softwares.com  login</v>
+      </c>
+      <c r="N18" t="str">
+        <v>developer@nex-softwares.com</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>Sun Aug 07 2022</v>
+      </c>
+      <c r="B19" t="str">
+        <v>11:47:32 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D19" t="str">
+        <v>User</v>
+      </c>
+      <c r="E19" t="str">
+        <v>/api/auth/login</v>
+      </c>
+      <c r="F19" t="str">
+        <v>login</v>
+      </c>
+      <c r="G19" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H19" t="str">
+        <v>developer@nex-softwares.com  login</v>
+      </c>
+      <c r="N19" t="str">
+        <v>developer@nex-softwares.com</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>Sun Aug 07 2022</v>
+      </c>
+      <c r="B20" t="str">
+        <v>13:34:06 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="C20" t="str">
+        <v>22892942601</v>
+      </c>
+      <c r="D20" t="str">
+        <v>User</v>
+      </c>
+      <c r="E20" t="str">
+        <v>/api/auth/send-otp</v>
+      </c>
+      <c r="F20" t="str">
+        <v>request</v>
+      </c>
+      <c r="G20" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H20" t="str">
+        <v>22892942601 request to receive otp</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>Sun Aug 07 2022</v>
+      </c>
+      <c r="B21" t="str">
+        <v>13:35:59 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="C21" t="str">
+        <v>22892942601</v>
+      </c>
+      <c r="D21" t="str">
+        <v>User</v>
+      </c>
+      <c r="E21" t="str">
+        <v>/api/auth/send-otp</v>
+      </c>
+      <c r="F21" t="str">
+        <v>request</v>
+      </c>
+      <c r="G21" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H21" t="str">
+        <v>22892942601 request to receive otp</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>Sun Aug 07 2022</v>
+      </c>
+      <c r="B22" t="str">
+        <v>13:36:12 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="C22" t="str">
+        <v>22892942601</v>
+      </c>
+      <c r="D22" t="str">
+        <v>User</v>
+      </c>
+      <c r="E22" t="str">
+        <v>/api/auth/verify-otp</v>
+      </c>
+      <c r="F22" t="str">
+        <v>request</v>
+      </c>
+      <c r="G22" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H22" t="str">
+        <v>22892942601 request to receive otp</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="K22" t="str">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>Sun Aug 07 2022</v>
+      </c>
+      <c r="B23" t="str">
+        <v>13:37:37 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D23" t="str">
+        <v>User</v>
+      </c>
+      <c r="E23" t="str">
+        <v>/api/auth/profile</v>
+      </c>
+      <c r="F23" t="str">
+        <v>read</v>
+      </c>
+      <c r="G23" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H23" t="str">
+        <v>Sonik  Kode  read his infos</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="K23" t="str">
+        <v>1</v>
+      </c>
+      <c r="L23" t="str">
+        <v>Sonik</v>
+      </c>
+      <c r="M23" t="str">
+        <v>Kode</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>Sun Aug 07 2022</v>
+      </c>
+      <c r="B24" t="str">
+        <v>13:50:28 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D24" t="str">
+        <v>User</v>
+      </c>
+      <c r="E24" t="str">
+        <v>/api/auth/id-card</v>
+      </c>
+      <c r="F24" t="str">
+        <v>upload</v>
+      </c>
+      <c r="G24" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H24" t="str">
+        <v>Sonik  Kode  upload his ID card</v>
+      </c>
+      <c r="I24" t="str">
+        <v>error.missing</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="K24" t="str">
+        <v>1</v>
+      </c>
+      <c r="L24" t="str">
+        <v>Sonik</v>
+      </c>
+      <c r="M24" t="str">
+        <v>Kode</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>Sun Aug 07 2022</v>
+      </c>
+      <c r="B25" t="str">
+        <v>13:53:27 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D25" t="str">
+        <v>User</v>
+      </c>
+      <c r="E25" t="str">
+        <v>/api/auth/id-card</v>
+      </c>
+      <c r="F25" t="str">
+        <v>upload</v>
+      </c>
+      <c r="G25" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H25" t="str">
+        <v>Sonik  Kode  upload his ID card</v>
+      </c>
+      <c r="I25" t="str">
+        <v>error.missing</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+      <c r="K25" t="str">
+        <v>1</v>
+      </c>
+      <c r="L25" t="str">
+        <v>Sonik</v>
+      </c>
+      <c r="M25" t="str">
+        <v>Kode</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>Sun Aug 07 2022</v>
+      </c>
+      <c r="B26" t="str">
+        <v>13:58:01 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D26" t="str">
+        <v>User</v>
+      </c>
+      <c r="E26" t="str">
+        <v>/api/auth/id-card</v>
+      </c>
+      <c r="F26" t="str">
+        <v>upload</v>
+      </c>
+      <c r="G26" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H26" t="str">
+        <v>Sonik  Kode  upload his ID card</v>
+      </c>
+      <c r="I26" t="str">
+        <v>error.missing</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="K26" t="str">
+        <v>1</v>
+      </c>
+      <c r="L26" t="str">
+        <v>Sonik</v>
+      </c>
+      <c r="M26" t="str">
+        <v>Kode</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>Sun Aug 07 2022</v>
+      </c>
+      <c r="B27" t="str">
+        <v>14:00:18 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D27" t="str">
+        <v>User</v>
+      </c>
+      <c r="E27" t="str">
+        <v>/api/auth/id-card</v>
+      </c>
+      <c r="F27" t="str">
+        <v>upload</v>
+      </c>
+      <c r="G27" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H27" t="str">
+        <v>Sonik  Kode  upload his ID card</v>
+      </c>
+      <c r="I27" t="str">
+        <v>Cannot read properties of undefined (reading 'idCard')</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27" t="str">
+        <v>1</v>
+      </c>
+      <c r="L27" t="str">
+        <v>Sonik</v>
+      </c>
+      <c r="M27" t="str">
+        <v>Kode</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>Sun Aug 07 2022</v>
+      </c>
+      <c r="B28" t="str">
+        <v>14:07:52 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D28" t="str">
+        <v>User</v>
+      </c>
+      <c r="E28" t="str">
+        <v>/api/auth/id-card</v>
+      </c>
+      <c r="F28" t="str">
+        <v>upload</v>
+      </c>
+      <c r="G28" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H28" t="str">
+        <v>Sonik  Kode  upload his ID card</v>
+      </c>
+      <c r="I28" t="str">
+        <v>error.missing</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28" t="str">
+        <v>1</v>
+      </c>
+      <c r="L28" t="str">
+        <v>Sonik</v>
+      </c>
+      <c r="M28" t="str">
+        <v>Kode</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>Sun Aug 07 2022</v>
+      </c>
+      <c r="B29" t="str">
+        <v>14:08:08 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D29" t="str">
+        <v>User</v>
+      </c>
+      <c r="E29" t="str">
+        <v>/api/auth/id-card</v>
+      </c>
+      <c r="F29" t="str">
+        <v>upload</v>
+      </c>
+      <c r="G29" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H29" t="str">
+        <v>Sonik  Kode  upload his ID card</v>
+      </c>
+      <c r="I29" t="str">
+        <v>error.missing</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="K29" t="str">
+        <v>1</v>
+      </c>
+      <c r="L29" t="str">
+        <v>Sonik</v>
+      </c>
+      <c r="M29" t="str">
+        <v>Kode</v>
+      </c>
+    </row>
+    <row r="30" xml:space="preserve">
+      <c r="A30" t="str">
+        <v>Sun Aug 07 2022</v>
+      </c>
+      <c r="B30" t="str">
+        <v>14:09:38 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D30" t="str">
+        <v>User</v>
+      </c>
+      <c r="E30" t="str">
+        <v>/api/auth/id-card</v>
+      </c>
+      <c r="F30" t="str">
+        <v>upload</v>
+      </c>
+      <c r="G30" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H30" t="str">
+        <v>Sonik  Kode  upload his ID card</v>
+      </c>
+      <c r="I30" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+Invalid `prisma.user.findFirst()` invocation:
+{
+  where: {
+    id: 1,
+    deletedAt: null
+  },
+  select: {
+    idCard: true,
+    ~~~~~~
+?   idCardStatus?: true,
+?   id?: true,
+?   countryId?: true,
+?   avatar?: true,
+?   email?: true,
+?   phoneNumber?: true,
+?   emailVerifiedAt?: true,
+?   phoneNumberVerifiedAt?: true,
+?   firstName?: true,
+?   lastName?: true,
+?   gender?: true,
+?   birthDay?: true,
+?   status?: true,
+?   role?: true,
+?   language?: true,
+?   idCardFront?: true,
+?   idCardBack?: true,
+?   idCardRejectionMessage?: true,
+?   idCardModifiedAt?: true,
+?   driverLicenseFront?: true,
+?   driverLicenseBack?: true,
+?   driverLicenseRejectionMessage?: true,
+?   driverLicenseStatus?: true,
+?   driverLicenseModifiedAt?: true,
+?   password?: true,
+?   rating?: true,
+?   createdAt?: true,
+?   blockedAt?: true,
+?   updatedAt?: true,
+?   profileCompletedAt?: true,
+?   deletedAt?: true,
+?   deletionReport?: true,
+?   preferences?: true,
+?   trips?: true,
+?   travels?: true,
+?   vehicles?: true,
+?   historics?: true,
+?   sendedNotifications?: true,
+?   receivedNotifications?: true,
+?   wallets?: true,
+?   devices?: true,
+?   payments?: true,
+?   country?: true,
+?   _count?: true
+  }
+}
+Unknown field `idCard` for select statement on model User. Available options are listed in green. Did you mean `id`?
+</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="K30" t="str">
+        <v>1</v>
+      </c>
+      <c r="L30" t="str">
+        <v>Sonik</v>
+      </c>
+      <c r="M30" t="str">
+        <v>Kode</v>
+      </c>
+    </row>
+    <row r="31" xml:space="preserve">
+      <c r="A31" t="str">
+        <v>Sun Aug 07 2022</v>
+      </c>
+      <c r="B31" t="str">
+        <v>14:10:31 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D31" t="str">
+        <v>User</v>
+      </c>
+      <c r="E31" t="str">
+        <v>/api/auth/id-card</v>
+      </c>
+      <c r="F31" t="str">
+        <v>upload</v>
+      </c>
+      <c r="G31" t="str">
+        <v>failed</v>
+      </c>
+      <c r="H31" t="str">
+        <v>Sonik  Kode  upload his ID card</v>
+      </c>
+      <c r="I31" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+Invalid `prisma.user.findFirst()` invocation:
+{
+  where: {
+    id: 1,
+    deletedAt: null
+  },
+  select: {
+    idCard: true,
+    ~~~~~~
+?   idCardStatus?: true,
+?   id?: true,
+?   countryId?: true,
+?   avatar?: true,
+?   email?: true,
+?   phoneNumber?: true,
+?   emailVerifiedAt?: true,
+?   phoneNumberVerifiedAt?: true,
+?   firstName?: true,
+?   lastName?: true,
+?   gender?: true,
+?   birthDay?: true,
+?   status?: true,
+?   role?: true,
+?   language?: true,
+?   idCardFront?: true,
+?   idCardBack?: true,
+?   idCardRejectionMessage?: true,
+?   idCardModifiedAt?: true,
+?   driverLicenseFront?: true,
+?   driverLicenseBack?: true,
+?   driverLicenseRejectionMessage?: true,
+?   driverLicenseStatus?: true,
+?   driverLicenseModifiedAt?: true,
+?   password?: true,
+?   rating?: true,
+?   createdAt?: true,
+?   blockedAt?: true,
+?   updatedAt?: true,
+?   profileCompletedAt?: true,
+?   deletedAt?: true,
+?   deletionReport?: true,
+?   preferences?: true,
+?   trips?: true,
+?   travels?: true,
+?   vehicles?: true,
+?   historics?: true,
+?   sendedNotifications?: true,
+?   receivedNotifications?: true,
+?   wallets?: true,
+?   devices?: true,
+?   payments?: true,
+?   country?: true,
+?   _count?: true
+  }
+}
+Unknown field `idCard` for select statement on model User. Available options are listed in green. Did you mean `id`?
+</v>
+      </c>
+      <c r="J31">
+        <v>1</v>
+      </c>
+      <c r="K31" t="str">
+        <v>1</v>
+      </c>
+      <c r="L31" t="str">
+        <v>Sonik</v>
+      </c>
+      <c r="M31" t="str">
+        <v>Kode</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>Sun Aug 07 2022</v>
+      </c>
+      <c r="B32" t="str">
+        <v>14:14:42 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D32" t="str">
+        <v>User</v>
+      </c>
+      <c r="E32" t="str">
+        <v>/api/auth/id-card</v>
+      </c>
+      <c r="F32" t="str">
+        <v>upload</v>
+      </c>
+      <c r="G32" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H32" t="str">
+        <v>Sonik  Kode  upload his ID card</v>
+      </c>
+      <c r="J32">
+        <v>1</v>
+      </c>
+      <c r="K32" t="str">
+        <v>1</v>
+      </c>
+      <c r="L32" t="str">
+        <v>Sonik</v>
+      </c>
+      <c r="M32" t="str">
+        <v>Kode</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>Sun Aug 07 2022</v>
+      </c>
+      <c r="B33" t="str">
+        <v>14:45:51 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D33" t="str">
+        <v>User</v>
+      </c>
+      <c r="E33" t="str">
+        <v>/api/auth/driver-license</v>
+      </c>
+      <c r="F33" t="str">
+        <v>upload</v>
+      </c>
+      <c r="G33" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H33" t="str">
+        <v>Sonik  Kode  upload his driver license</v>
+      </c>
+      <c r="J33">
+        <v>1</v>
+      </c>
+      <c r="K33" t="str">
+        <v>1</v>
+      </c>
+      <c r="L33" t="str">
+        <v>Sonik</v>
+      </c>
+      <c r="M33" t="str">
+        <v>Kode</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>Sun Aug 07 2022</v>
+      </c>
+      <c r="B34" t="str">
+        <v>14:47:35 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D34" t="str">
+        <v>User</v>
+      </c>
+      <c r="E34" t="str">
+        <v>/api/auth/upload-document</v>
+      </c>
+      <c r="F34" t="str">
+        <v>upload</v>
+      </c>
+      <c r="G34" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H34" t="str">
+        <v>Sonik  Kode  upload his documents</v>
+      </c>
+      <c r="J34">
+        <v>1</v>
+      </c>
+      <c r="K34" t="str">
+        <v>1</v>
+      </c>
+      <c r="L34" t="str">
+        <v>Sonik</v>
+      </c>
+      <c r="M34" t="str">
+        <v>Kode</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>Mon Aug 08 2022</v>
+      </c>
+      <c r="B35" t="str">
+        <v>02:00:21 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D35" t="str">
+        <v>User</v>
+      </c>
+      <c r="E35" t="str">
+        <v>/api/auth/login</v>
+      </c>
+      <c r="F35" t="str">
+        <v>login</v>
+      </c>
+      <c r="G35" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H35" t="str">
+        <v>developer@nex-softwares.com  login</v>
+      </c>
+      <c r="N35" t="str">
+        <v>developer@nex-softwares.com</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:N35"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add withdrawal use case
</commit_message>
<xml_diff>
--- a/user-logs/data.xlsx
+++ b/user-logs/data.xlsx
@@ -14288,7 +14288,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N35"/>
+  <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -15533,9 +15533,525 @@
         <v>developer@nex-softwares.com</v>
       </c>
     </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>Tue Aug 23 2022</v>
+      </c>
+      <c r="B36" t="str">
+        <v>16:08:34 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D36" t="str">
+        <v>User</v>
+      </c>
+      <c r="E36" t="str">
+        <v>/api/auth/login</v>
+      </c>
+      <c r="F36" t="str">
+        <v>login</v>
+      </c>
+      <c r="G36" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H36" t="str">
+        <v>developer@nex-softwares.com  login</v>
+      </c>
+      <c r="N36" t="str">
+        <v>developer@nex-softwares.com</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>Tue Aug 23 2022</v>
+      </c>
+      <c r="B37" t="str">
+        <v>16:08:35 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D37" t="str">
+        <v>User</v>
+      </c>
+      <c r="E37" t="str">
+        <v>/api/user</v>
+      </c>
+      <c r="F37" t="str">
+        <v>read</v>
+      </c>
+      <c r="G37" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H37" t="str">
+        <v>NEX  Admin  read all users (4) from 0 to 100</v>
+      </c>
+      <c r="J37">
+        <v>9</v>
+      </c>
+      <c r="K37" t="str">
+        <v>all</v>
+      </c>
+      <c r="L37" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="M37" t="str">
+        <v>Admin</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>Tue Aug 23 2022</v>
+      </c>
+      <c r="B38" t="str">
+        <v>16:08:38 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D38" t="str">
+        <v>User</v>
+      </c>
+      <c r="E38" t="str">
+        <v>/api/user</v>
+      </c>
+      <c r="F38" t="str">
+        <v>read</v>
+      </c>
+      <c r="G38" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H38" t="str">
+        <v>NEX  Admin  read all users (4) from 0 to 100</v>
+      </c>
+      <c r="J38">
+        <v>9</v>
+      </c>
+      <c r="K38" t="str">
+        <v>all</v>
+      </c>
+      <c r="L38" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="M38" t="str">
+        <v>Admin</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>Tue Aug 23 2022</v>
+      </c>
+      <c r="B39" t="str">
+        <v>16:08:53 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D39" t="str">
+        <v>User</v>
+      </c>
+      <c r="E39" t="str">
+        <v>/api/to-validate-users</v>
+      </c>
+      <c r="F39" t="str">
+        <v>read</v>
+      </c>
+      <c r="G39" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H39" t="str">
+        <v>NEX  Admin  read all to validate users (1) from 0 to 100</v>
+      </c>
+      <c r="J39">
+        <v>9</v>
+      </c>
+      <c r="K39" t="str">
+        <v>all</v>
+      </c>
+      <c r="L39" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="M39" t="str">
+        <v>Admin</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>Tue Aug 23 2022</v>
+      </c>
+      <c r="B40" t="str">
+        <v>16:09:11 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D40" t="str">
+        <v>Trip</v>
+      </c>
+      <c r="E40" t="str">
+        <v>/api/trip</v>
+      </c>
+      <c r="F40" t="str">
+        <v>read</v>
+      </c>
+      <c r="G40" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H40" t="str">
+        <v>NEX  Admin  read all trips (2) from 0 to 100</v>
+      </c>
+      <c r="J40">
+        <v>9</v>
+      </c>
+      <c r="K40" t="str">
+        <v>all</v>
+      </c>
+      <c r="L40" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="M40" t="str">
+        <v>Admin</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>Tue Aug 23 2022</v>
+      </c>
+      <c r="B41" t="str">
+        <v>16:09:18 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D41" t="str">
+        <v>Preference</v>
+      </c>
+      <c r="E41" t="str">
+        <v>/api/preference</v>
+      </c>
+      <c r="F41" t="str">
+        <v>read</v>
+      </c>
+      <c r="G41" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H41" t="str">
+        <v>NEX  Admin  read all preferences (undefined) from undefined to NaN</v>
+      </c>
+      <c r="J41">
+        <v>9</v>
+      </c>
+      <c r="K41" t="str">
+        <v>all</v>
+      </c>
+      <c r="L41" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="M41" t="str">
+        <v>Admin</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>Tue Aug 23 2022</v>
+      </c>
+      <c r="B42" t="str">
+        <v>16:09:22 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D42" t="str">
+        <v>VehicleType</v>
+      </c>
+      <c r="E42" t="str">
+        <v>/api/vehicle-type</v>
+      </c>
+      <c r="F42" t="str">
+        <v>read</v>
+      </c>
+      <c r="G42" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H42" t="str">
+        <v>NEX  Admin  read all vehicle types (undefined) from undefined to NaN</v>
+      </c>
+      <c r="J42">
+        <v>9</v>
+      </c>
+      <c r="K42" t="str">
+        <v>all</v>
+      </c>
+      <c r="L42" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="M42" t="str">
+        <v>Admin</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>Tue Aug 23 2022</v>
+      </c>
+      <c r="B43" t="str">
+        <v>16:09:27 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D43" t="str">
+        <v>Pricing</v>
+      </c>
+      <c r="E43" t="str">
+        <v>/api/pricing</v>
+      </c>
+      <c r="F43" t="str">
+        <v>read</v>
+      </c>
+      <c r="G43" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H43" t="str">
+        <v>NEX  Admin  read all pricing (undefined) from undefined to NaN</v>
+      </c>
+      <c r="J43">
+        <v>9</v>
+      </c>
+      <c r="K43" t="str">
+        <v>all</v>
+      </c>
+      <c r="L43" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="M43" t="str">
+        <v>Admin</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>Tue Aug 23 2022</v>
+      </c>
+      <c r="B44" t="str">
+        <v>16:09:51 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D44" t="str">
+        <v>VehicleType</v>
+      </c>
+      <c r="E44" t="str">
+        <v>/api/vehicle-type</v>
+      </c>
+      <c r="F44" t="str">
+        <v>read</v>
+      </c>
+      <c r="G44" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H44" t="str">
+        <v>NEX  Admin  read all vehicle types (undefined) from undefined to NaN</v>
+      </c>
+      <c r="J44">
+        <v>9</v>
+      </c>
+      <c r="K44" t="str">
+        <v>all</v>
+      </c>
+      <c r="L44" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="M44" t="str">
+        <v>Admin</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>Tue Aug 23 2022</v>
+      </c>
+      <c r="B45" t="str">
+        <v>16:09:55 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D45" t="str">
+        <v>Trip</v>
+      </c>
+      <c r="E45" t="str">
+        <v>/api/trip</v>
+      </c>
+      <c r="F45" t="str">
+        <v>read</v>
+      </c>
+      <c r="G45" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H45" t="str">
+        <v>NEX  Admin  read all trips (2) from 0 to 100</v>
+      </c>
+      <c r="J45">
+        <v>9</v>
+      </c>
+      <c r="K45" t="str">
+        <v>all</v>
+      </c>
+      <c r="L45" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="M45" t="str">
+        <v>Admin</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>Tue Aug 23 2022</v>
+      </c>
+      <c r="B46" t="str">
+        <v>16:41:59 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D46" t="str">
+        <v>Trip</v>
+      </c>
+      <c r="E46" t="str">
+        <v>/api/trip</v>
+      </c>
+      <c r="F46" t="str">
+        <v>read</v>
+      </c>
+      <c r="G46" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H46" t="str">
+        <v>NEX  Admin  read all trips (2) from 0 to 100</v>
+      </c>
+      <c r="J46">
+        <v>9</v>
+      </c>
+      <c r="K46" t="str">
+        <v>all</v>
+      </c>
+      <c r="L46" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="M46" t="str">
+        <v>Admin</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>Tue Aug 23 2022</v>
+      </c>
+      <c r="B47" t="str">
+        <v>21:29:18 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D47" t="str">
+        <v>User</v>
+      </c>
+      <c r="E47" t="str">
+        <v>/api/user</v>
+      </c>
+      <c r="F47" t="str">
+        <v>read</v>
+      </c>
+      <c r="G47" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H47" t="str">
+        <v>NEX  Admin  read all users (4) from 0 to 100</v>
+      </c>
+      <c r="J47">
+        <v>9</v>
+      </c>
+      <c r="K47" t="str">
+        <v>all</v>
+      </c>
+      <c r="L47" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="M47" t="str">
+        <v>Admin</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>Tue Aug 23 2022</v>
+      </c>
+      <c r="B48" t="str">
+        <v>21:38:30 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D48" t="str">
+        <v>Trip</v>
+      </c>
+      <c r="E48" t="str">
+        <v>/api/trip</v>
+      </c>
+      <c r="F48" t="str">
+        <v>read</v>
+      </c>
+      <c r="G48" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H48" t="str">
+        <v>NEX  Admin  read all trips (2) from 0 to 100</v>
+      </c>
+      <c r="J48">
+        <v>9</v>
+      </c>
+      <c r="K48" t="str">
+        <v>all</v>
+      </c>
+      <c r="L48" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="M48" t="str">
+        <v>Admin</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>Tue Aug 23 2022</v>
+      </c>
+      <c r="B49" t="str">
+        <v>21:38:39 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D49" t="str">
+        <v>Trip</v>
+      </c>
+      <c r="E49" t="str">
+        <v>/api/trip</v>
+      </c>
+      <c r="F49" t="str">
+        <v>read</v>
+      </c>
+      <c r="G49" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H49" t="str">
+        <v>NEX  Admin  read all trips (2) from 0 to 100</v>
+      </c>
+      <c r="J49">
+        <v>9</v>
+      </c>
+      <c r="K49" t="str">
+        <v>all</v>
+      </c>
+      <c r="L49" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="M49" t="str">
+        <v>Admin</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>Tue Aug 23 2022</v>
+      </c>
+      <c r="B50" t="str">
+        <v>21:38:40 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D50" t="str">
+        <v>User</v>
+      </c>
+      <c r="E50" t="str">
+        <v>/api/to-validate-users</v>
+      </c>
+      <c r="F50" t="str">
+        <v>read</v>
+      </c>
+      <c r="G50" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H50" t="str">
+        <v>NEX  Admin  read all to validate users (1) from 0 to 100</v>
+      </c>
+      <c r="J50">
+        <v>9</v>
+      </c>
+      <c r="K50" t="str">
+        <v>all</v>
+      </c>
+      <c r="L50" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="M50" t="str">
+        <v>Admin</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N35"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N50"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
return prefrences in profile
</commit_message>
<xml_diff>
--- a/user-logs/data.xlsx
+++ b/user-logs/data.xlsx
@@ -10,6 +10,7 @@
     <sheet name="2022_5" sheetId="5" r:id="rId5"/>
     <sheet name="2022_7" sheetId="6" r:id="rId6"/>
     <sheet name="2022_8" sheetId="7" r:id="rId7"/>
+    <sheet name="2022_9" sheetId="8" r:id="rId8"/>
   </sheets>
 </workbook>
 </file>
@@ -16054,4 +16055,2538 @@
     <ignoredError numberStoredAsText="1" sqref="A1:N50"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L72"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>date</v>
+      </c>
+      <c r="B1" t="str">
+        <v>time</v>
+      </c>
+      <c r="C1" t="str">
+        <v>email</v>
+      </c>
+      <c r="D1" t="str">
+        <v>model</v>
+      </c>
+      <c r="E1" t="str">
+        <v>path</v>
+      </c>
+      <c r="F1" t="str">
+        <v>action</v>
+      </c>
+      <c r="G1" t="str">
+        <v>status</v>
+      </c>
+      <c r="H1" t="str">
+        <v>description</v>
+      </c>
+      <c r="I1" t="str">
+        <v>userId</v>
+      </c>
+      <c r="J1" t="str">
+        <v>lastName</v>
+      </c>
+      <c r="K1" t="str">
+        <v>firstName</v>
+      </c>
+      <c r="L1" t="str">
+        <v>modelId</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B2" t="str">
+        <v>03:15:40 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="C2" t="str">
+        <v>developer@nex-softwares.com</v>
+      </c>
+      <c r="D2" t="str">
+        <v>User</v>
+      </c>
+      <c r="E2" t="str">
+        <v>/api/auth/login</v>
+      </c>
+      <c r="F2" t="str">
+        <v>login</v>
+      </c>
+      <c r="G2" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H2" t="str">
+        <v>developer@nex-softwares.com  login</v>
+      </c>
+      <c r="I2" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="J2" t="str">
+        <v>developer@nex-softwares.com  login</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B3" t="str">
+        <v>03:15:41 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D3" t="str">
+        <v>User</v>
+      </c>
+      <c r="E3" t="str">
+        <v>/api/user</v>
+      </c>
+      <c r="F3" t="str">
+        <v>read</v>
+      </c>
+      <c r="G3" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H3" t="str">
+        <v>NEX  Admin  read all users (4) from 0 to 100</v>
+      </c>
+      <c r="I3">
+        <v>9</v>
+      </c>
+      <c r="J3" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K3" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L3" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B4" t="str">
+        <v>03:15:44 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Preference</v>
+      </c>
+      <c r="E4" t="str">
+        <v>/api/preference</v>
+      </c>
+      <c r="F4" t="str">
+        <v>read</v>
+      </c>
+      <c r="G4" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H4" t="str">
+        <v>NEX  Admin  read all preferences (undefined) from undefined to NaN</v>
+      </c>
+      <c r="I4">
+        <v>9</v>
+      </c>
+      <c r="J4" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K4" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L4" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B5" t="str">
+        <v>03:15:47 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D5" t="str">
+        <v>VehicleType</v>
+      </c>
+      <c r="E5" t="str">
+        <v>/api/vehicle-type</v>
+      </c>
+      <c r="F5" t="str">
+        <v>read</v>
+      </c>
+      <c r="G5" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H5" t="str">
+        <v>NEX  Admin  read all vehicle types (undefined) from undefined to NaN</v>
+      </c>
+      <c r="I5">
+        <v>9</v>
+      </c>
+      <c r="J5" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K5" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L5" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B6" t="str">
+        <v>03:15:50 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D6" t="str">
+        <v>Pricing</v>
+      </c>
+      <c r="E6" t="str">
+        <v>/api/pricing</v>
+      </c>
+      <c r="F6" t="str">
+        <v>read</v>
+      </c>
+      <c r="G6" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H6" t="str">
+        <v>NEX  Admin  read all pricing (undefined) from undefined to NaN</v>
+      </c>
+      <c r="I6">
+        <v>9</v>
+      </c>
+      <c r="J6" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K6" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L6" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B7" t="str">
+        <v>03:16:48 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D7" t="str">
+        <v>User</v>
+      </c>
+      <c r="E7" t="str">
+        <v>/api/to-validate-users</v>
+      </c>
+      <c r="F7" t="str">
+        <v>read</v>
+      </c>
+      <c r="G7" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H7" t="str">
+        <v>NEX  Admin  read all to validate users (1) from 0 to 100</v>
+      </c>
+      <c r="I7">
+        <v>9</v>
+      </c>
+      <c r="J7" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K7" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L7" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B8" t="str">
+        <v>03:17:00 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D8" t="str">
+        <v>User</v>
+      </c>
+      <c r="E8" t="str">
+        <v>/api/to-validate-users</v>
+      </c>
+      <c r="F8" t="str">
+        <v>read</v>
+      </c>
+      <c r="G8" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H8" t="str">
+        <v>NEX  Admin  read all to validate users (1) from 0 to 100</v>
+      </c>
+      <c r="I8">
+        <v>9</v>
+      </c>
+      <c r="J8" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K8" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L8" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B9" t="str">
+        <v>03:17:02 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D9" t="str">
+        <v>User</v>
+      </c>
+      <c r="E9" t="str">
+        <v>/api/user</v>
+      </c>
+      <c r="F9" t="str">
+        <v>read</v>
+      </c>
+      <c r="G9" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H9" t="str">
+        <v>NEX  Admin  read all users (4) from 0 to 100</v>
+      </c>
+      <c r="I9">
+        <v>9</v>
+      </c>
+      <c r="J9" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K9" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L9" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B10" t="str">
+        <v>03:17:03 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D10" t="str">
+        <v>Trip</v>
+      </c>
+      <c r="E10" t="str">
+        <v>/api/trip</v>
+      </c>
+      <c r="F10" t="str">
+        <v>read</v>
+      </c>
+      <c r="G10" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H10" t="str">
+        <v>NEX  Admin  read all trips (2) from 0 to 100</v>
+      </c>
+      <c r="I10">
+        <v>9</v>
+      </c>
+      <c r="J10" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K10" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L10" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B11" t="str">
+        <v>03:17:28 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D11" t="str">
+        <v>Trip</v>
+      </c>
+      <c r="E11" t="str">
+        <v>/api/trip</v>
+      </c>
+      <c r="F11" t="str">
+        <v>read</v>
+      </c>
+      <c r="G11" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H11" t="str">
+        <v>NEX  Admin  read all trips (2) from 0 to 100</v>
+      </c>
+      <c r="I11">
+        <v>9</v>
+      </c>
+      <c r="J11" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K11" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L11" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B12" t="str">
+        <v>03:19:20 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D12" t="str">
+        <v>User</v>
+      </c>
+      <c r="E12" t="str">
+        <v>/api/to-validate-users</v>
+      </c>
+      <c r="F12" t="str">
+        <v>read</v>
+      </c>
+      <c r="G12" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H12" t="str">
+        <v>NEX  Admin  read all to validate users (1) from 0 to 100</v>
+      </c>
+      <c r="I12">
+        <v>9</v>
+      </c>
+      <c r="J12" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K12" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L12" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B13" t="str">
+        <v>03:19:22 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D13" t="str">
+        <v>Trip</v>
+      </c>
+      <c r="E13" t="str">
+        <v>/api/trip</v>
+      </c>
+      <c r="F13" t="str">
+        <v>read</v>
+      </c>
+      <c r="G13" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H13" t="str">
+        <v>NEX  Admin  read all trips (2) from 0 to 100</v>
+      </c>
+      <c r="I13">
+        <v>9</v>
+      </c>
+      <c r="J13" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K13" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L13" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B14" t="str">
+        <v>03:44:10 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D14" t="str">
+        <v>Trip</v>
+      </c>
+      <c r="E14" t="str">
+        <v>/api/trip</v>
+      </c>
+      <c r="F14" t="str">
+        <v>read</v>
+      </c>
+      <c r="G14" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H14" t="str">
+        <v>NEX  Admin  read all trips (2) from 0 to 100</v>
+      </c>
+      <c r="I14">
+        <v>9</v>
+      </c>
+      <c r="J14" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K14" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L14" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B15" t="str">
+        <v>03:45:27 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D15" t="str">
+        <v>Preference</v>
+      </c>
+      <c r="E15" t="str">
+        <v>/api/preference</v>
+      </c>
+      <c r="F15" t="str">
+        <v>read</v>
+      </c>
+      <c r="G15" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H15" t="str">
+        <v>NEX  Admin  read all preferences (undefined) from undefined to NaN</v>
+      </c>
+      <c r="I15">
+        <v>9</v>
+      </c>
+      <c r="J15" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K15" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L15" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B16" t="str">
+        <v>03:45:30 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D16" t="str">
+        <v>Pricing</v>
+      </c>
+      <c r="E16" t="str">
+        <v>/api/pricing</v>
+      </c>
+      <c r="F16" t="str">
+        <v>read</v>
+      </c>
+      <c r="G16" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H16" t="str">
+        <v>NEX  Admin  read all pricing (undefined) from undefined to NaN</v>
+      </c>
+      <c r="I16">
+        <v>9</v>
+      </c>
+      <c r="J16" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K16" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L16" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B17" t="str">
+        <v>03:46:35 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D17" t="str">
+        <v>User</v>
+      </c>
+      <c r="E17" t="str">
+        <v>/api/user</v>
+      </c>
+      <c r="F17" t="str">
+        <v>read</v>
+      </c>
+      <c r="G17" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H17" t="str">
+        <v>NEX  Admin  read all users (4) from 0 to 100</v>
+      </c>
+      <c r="I17">
+        <v>9</v>
+      </c>
+      <c r="J17" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K17" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L17" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B18" t="str">
+        <v>03:46:41 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D18" t="str">
+        <v>Preference</v>
+      </c>
+      <c r="E18" t="str">
+        <v>/api/preference</v>
+      </c>
+      <c r="F18" t="str">
+        <v>read</v>
+      </c>
+      <c r="G18" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H18" t="str">
+        <v>NEX  Admin  read all preferences (undefined) from undefined to NaN</v>
+      </c>
+      <c r="I18">
+        <v>9</v>
+      </c>
+      <c r="J18" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K18" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L18" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B19" t="str">
+        <v>03:46:44 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D19" t="str">
+        <v>Trip</v>
+      </c>
+      <c r="E19" t="str">
+        <v>/api/trip</v>
+      </c>
+      <c r="F19" t="str">
+        <v>read</v>
+      </c>
+      <c r="G19" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H19" t="str">
+        <v>NEX  Admin  read all trips (2) from 0 to 100</v>
+      </c>
+      <c r="I19">
+        <v>9</v>
+      </c>
+      <c r="J19" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K19" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L19" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B20" t="str">
+        <v>03:47:51 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D20" t="str">
+        <v>User</v>
+      </c>
+      <c r="E20" t="str">
+        <v>/api/to-validate-users</v>
+      </c>
+      <c r="F20" t="str">
+        <v>read</v>
+      </c>
+      <c r="G20" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H20" t="str">
+        <v>NEX  Admin  read all to validate users (1) from 0 to 100</v>
+      </c>
+      <c r="I20">
+        <v>9</v>
+      </c>
+      <c r="J20" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K20" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L20" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B21" t="str">
+        <v>03:47:53 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D21" t="str">
+        <v>Trip</v>
+      </c>
+      <c r="E21" t="str">
+        <v>/api/trip</v>
+      </c>
+      <c r="F21" t="str">
+        <v>read</v>
+      </c>
+      <c r="G21" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H21" t="str">
+        <v>NEX  Admin  read all trips (2) from 0 to 100</v>
+      </c>
+      <c r="I21">
+        <v>9</v>
+      </c>
+      <c r="J21" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K21" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L21" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B22" t="str">
+        <v>03:49:28 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D22" t="str">
+        <v>Trip</v>
+      </c>
+      <c r="E22" t="str">
+        <v>/api/trip</v>
+      </c>
+      <c r="F22" t="str">
+        <v>read</v>
+      </c>
+      <c r="G22" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H22" t="str">
+        <v>NEX  Admin  read all trips (2) from 0 to 100</v>
+      </c>
+      <c r="I22">
+        <v>9</v>
+      </c>
+      <c r="J22" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K22" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L22" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B23" t="str">
+        <v>03:51:21 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D23" t="str">
+        <v>Trip</v>
+      </c>
+      <c r="E23" t="str">
+        <v>/api/trip</v>
+      </c>
+      <c r="F23" t="str">
+        <v>read</v>
+      </c>
+      <c r="G23" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H23" t="str">
+        <v>NEX  Admin  read all trips (2) from 0 to 100</v>
+      </c>
+      <c r="I23">
+        <v>9</v>
+      </c>
+      <c r="J23" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K23" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L23" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B24" t="str">
+        <v>03:52:55 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D24" t="str">
+        <v>Trip</v>
+      </c>
+      <c r="E24" t="str">
+        <v>/api/trip</v>
+      </c>
+      <c r="F24" t="str">
+        <v>read</v>
+      </c>
+      <c r="G24" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H24" t="str">
+        <v>NEX  Admin  read all trips (2) from 0 to 100</v>
+      </c>
+      <c r="I24">
+        <v>9</v>
+      </c>
+      <c r="J24" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K24" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L24" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B25" t="str">
+        <v>03:54:27 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D25" t="str">
+        <v>User</v>
+      </c>
+      <c r="E25" t="str">
+        <v>/api/user</v>
+      </c>
+      <c r="F25" t="str">
+        <v>read</v>
+      </c>
+      <c r="G25" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H25" t="str">
+        <v>NEX  Admin  read all users (4) from 0 to 100</v>
+      </c>
+      <c r="I25">
+        <v>9</v>
+      </c>
+      <c r="J25" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K25" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L25" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B26" t="str">
+        <v>03:54:28 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D26" t="str">
+        <v>User</v>
+      </c>
+      <c r="E26" t="str">
+        <v>/api/user</v>
+      </c>
+      <c r="F26" t="str">
+        <v>read</v>
+      </c>
+      <c r="G26" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H26" t="str">
+        <v>NEX  Admin  read all users (4) from 0 to 100</v>
+      </c>
+      <c r="I26">
+        <v>9</v>
+      </c>
+      <c r="J26" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K26" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L26" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B27" t="str">
+        <v>03:54:29 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D27" t="str">
+        <v>User</v>
+      </c>
+      <c r="E27" t="str">
+        <v>/api/to-validate-users</v>
+      </c>
+      <c r="F27" t="str">
+        <v>read</v>
+      </c>
+      <c r="G27" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H27" t="str">
+        <v>NEX  Admin  read all to validate users (1) from 0 to 100</v>
+      </c>
+      <c r="I27">
+        <v>9</v>
+      </c>
+      <c r="J27" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K27" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L27" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B28" t="str">
+        <v>03:54:31 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D28" t="str">
+        <v>User</v>
+      </c>
+      <c r="E28" t="str">
+        <v>/api/user</v>
+      </c>
+      <c r="F28" t="str">
+        <v>read</v>
+      </c>
+      <c r="G28" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H28" t="str">
+        <v>NEX  Admin  read all users (4) from 0 to 100</v>
+      </c>
+      <c r="I28">
+        <v>9</v>
+      </c>
+      <c r="J28" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K28" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L28" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B29" t="str">
+        <v>03:54:32 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D29" t="str">
+        <v>User</v>
+      </c>
+      <c r="E29" t="str">
+        <v>/api/user</v>
+      </c>
+      <c r="F29" t="str">
+        <v>read</v>
+      </c>
+      <c r="G29" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H29" t="str">
+        <v>NEX  Admin  read all users (4) from 0 to 100</v>
+      </c>
+      <c r="I29">
+        <v>9</v>
+      </c>
+      <c r="J29" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K29" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L29" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B30" t="str">
+        <v>03:54:32 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D30" t="str">
+        <v>User</v>
+      </c>
+      <c r="E30" t="str">
+        <v>/api/to-validate-users</v>
+      </c>
+      <c r="F30" t="str">
+        <v>read</v>
+      </c>
+      <c r="G30" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H30" t="str">
+        <v>NEX  Admin  read all to validate users (1) from 0 to 100</v>
+      </c>
+      <c r="I30">
+        <v>9</v>
+      </c>
+      <c r="J30" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K30" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L30" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B31" t="str">
+        <v>03:54:33 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D31" t="str">
+        <v>Trip</v>
+      </c>
+      <c r="E31" t="str">
+        <v>/api/trip</v>
+      </c>
+      <c r="F31" t="str">
+        <v>read</v>
+      </c>
+      <c r="G31" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H31" t="str">
+        <v>NEX  Admin  read all trips (2) from 0 to 100</v>
+      </c>
+      <c r="I31">
+        <v>9</v>
+      </c>
+      <c r="J31" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K31" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L31" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B32" t="str">
+        <v>04:02:42 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D32" t="str">
+        <v>User</v>
+      </c>
+      <c r="E32" t="str">
+        <v>/api/user</v>
+      </c>
+      <c r="F32" t="str">
+        <v>read</v>
+      </c>
+      <c r="G32" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H32" t="str">
+        <v>NEX  Admin  read all users (4) from 0 to 100</v>
+      </c>
+      <c r="I32">
+        <v>9</v>
+      </c>
+      <c r="J32" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K32" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L32" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B33" t="str">
+        <v>04:05:37 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D33" t="str">
+        <v>Trip</v>
+      </c>
+      <c r="E33" t="str">
+        <v>/api/trip</v>
+      </c>
+      <c r="F33" t="str">
+        <v>read</v>
+      </c>
+      <c r="G33" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H33" t="str">
+        <v>NEX  Admin  read all trips (2) from 0 to 100</v>
+      </c>
+      <c r="I33">
+        <v>9</v>
+      </c>
+      <c r="J33" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K33" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L33" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B34" t="str">
+        <v>04:23:55 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D34" t="str">
+        <v>User</v>
+      </c>
+      <c r="E34" t="str">
+        <v>/api/user</v>
+      </c>
+      <c r="F34" t="str">
+        <v>read</v>
+      </c>
+      <c r="G34" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H34" t="str">
+        <v>NEX  Admin  read all users (4) from 0 to 100</v>
+      </c>
+      <c r="I34">
+        <v>9</v>
+      </c>
+      <c r="J34" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K34" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L34" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B35" t="str">
+        <v>04:28:47 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D35" t="str">
+        <v>User</v>
+      </c>
+      <c r="E35" t="str">
+        <v>/api/user</v>
+      </c>
+      <c r="F35" t="str">
+        <v>read</v>
+      </c>
+      <c r="G35" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H35" t="str">
+        <v>NEX  Admin  read all users (4) from 0 to 100</v>
+      </c>
+      <c r="I35">
+        <v>9</v>
+      </c>
+      <c r="J35" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K35" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L35" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B36" t="str">
+        <v>04:29:37 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D36" t="str">
+        <v>User</v>
+      </c>
+      <c r="E36" t="str">
+        <v>/api/user</v>
+      </c>
+      <c r="F36" t="str">
+        <v>read</v>
+      </c>
+      <c r="G36" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H36" t="str">
+        <v>NEX  Admin  read all users (4) from 0 to 100</v>
+      </c>
+      <c r="I36">
+        <v>9</v>
+      </c>
+      <c r="J36" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K36" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L36" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B37" t="str">
+        <v>04:37:31 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D37" t="str">
+        <v>User</v>
+      </c>
+      <c r="E37" t="str">
+        <v>/api/to-validate-users</v>
+      </c>
+      <c r="F37" t="str">
+        <v>read</v>
+      </c>
+      <c r="G37" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H37" t="str">
+        <v>NEX  Admin  read all to validate users (1) from 0 to 100</v>
+      </c>
+      <c r="I37">
+        <v>9</v>
+      </c>
+      <c r="J37" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K37" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L37" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B38" t="str">
+        <v>04:37:32 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D38" t="str">
+        <v>User</v>
+      </c>
+      <c r="E38" t="str">
+        <v>/api/user</v>
+      </c>
+      <c r="F38" t="str">
+        <v>read</v>
+      </c>
+      <c r="G38" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H38" t="str">
+        <v>NEX  Admin  read all users (4) from 0 to 100</v>
+      </c>
+      <c r="I38">
+        <v>9</v>
+      </c>
+      <c r="J38" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K38" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L38" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B39" t="str">
+        <v>04:37:33 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D39" t="str">
+        <v>User</v>
+      </c>
+      <c r="E39" t="str">
+        <v>/api/to-validate-users</v>
+      </c>
+      <c r="F39" t="str">
+        <v>read</v>
+      </c>
+      <c r="G39" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H39" t="str">
+        <v>NEX  Admin  read all to validate users (1) from 0 to 100</v>
+      </c>
+      <c r="I39">
+        <v>9</v>
+      </c>
+      <c r="J39" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K39" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L39" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B40" t="str">
+        <v>04:39:15 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D40" t="str">
+        <v>User</v>
+      </c>
+      <c r="E40" t="str">
+        <v>/api/to-validate-users</v>
+      </c>
+      <c r="F40" t="str">
+        <v>read</v>
+      </c>
+      <c r="G40" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H40" t="str">
+        <v>NEX  Admin  read all to validate users (1) from 0 to 100</v>
+      </c>
+      <c r="I40">
+        <v>9</v>
+      </c>
+      <c r="J40" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K40" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L40" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B41" t="str">
+        <v>04:39:17 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D41" t="str">
+        <v>Trip</v>
+      </c>
+      <c r="E41" t="str">
+        <v>/api/trip</v>
+      </c>
+      <c r="F41" t="str">
+        <v>read</v>
+      </c>
+      <c r="G41" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H41" t="str">
+        <v>NEX  Admin  read all trips (2) from 0 to 100</v>
+      </c>
+      <c r="I41">
+        <v>9</v>
+      </c>
+      <c r="J41" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K41" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L41" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B42" t="str">
+        <v>04:39:24 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D42" t="str">
+        <v>Trip</v>
+      </c>
+      <c r="E42" t="str">
+        <v>/api/trip</v>
+      </c>
+      <c r="F42" t="str">
+        <v>read</v>
+      </c>
+      <c r="G42" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H42" t="str">
+        <v>NEX  Admin  read all trips (2) from 0 to 100</v>
+      </c>
+      <c r="I42">
+        <v>9</v>
+      </c>
+      <c r="J42" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K42" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L42" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B43" t="str">
+        <v>05:02:16 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D43" t="str">
+        <v>Trip</v>
+      </c>
+      <c r="E43" t="str">
+        <v>/api/trip</v>
+      </c>
+      <c r="F43" t="str">
+        <v>read</v>
+      </c>
+      <c r="G43" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H43" t="str">
+        <v>NEX  Admin  read all trips (2) from 0 to 100</v>
+      </c>
+      <c r="I43">
+        <v>9</v>
+      </c>
+      <c r="J43" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K43" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L43" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B44" t="str">
+        <v>05:02:20 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D44" t="str">
+        <v>User</v>
+      </c>
+      <c r="E44" t="str">
+        <v>/api/to-validate-users</v>
+      </c>
+      <c r="F44" t="str">
+        <v>read</v>
+      </c>
+      <c r="G44" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H44" t="str">
+        <v>NEX  Admin  read all to validate users (1) from 0 to 100</v>
+      </c>
+      <c r="I44">
+        <v>9</v>
+      </c>
+      <c r="J44" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K44" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L44" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B45" t="str">
+        <v>05:02:23 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D45" t="str">
+        <v>Trip</v>
+      </c>
+      <c r="E45" t="str">
+        <v>/api/trip</v>
+      </c>
+      <c r="F45" t="str">
+        <v>read</v>
+      </c>
+      <c r="G45" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H45" t="str">
+        <v>NEX  Admin  read all trips (2) from 0 to 100</v>
+      </c>
+      <c r="I45">
+        <v>9</v>
+      </c>
+      <c r="J45" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K45" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L45" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B46" t="str">
+        <v>05:10:21 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D46" t="str">
+        <v>Trip</v>
+      </c>
+      <c r="E46" t="str">
+        <v>/api/trip</v>
+      </c>
+      <c r="F46" t="str">
+        <v>read</v>
+      </c>
+      <c r="G46" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H46" t="str">
+        <v>NEX  Admin  read all trips (2) from 0 to 100</v>
+      </c>
+      <c r="I46">
+        <v>9</v>
+      </c>
+      <c r="J46" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K46" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L46" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B47" t="str">
+        <v>05:12:32 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D47" t="str">
+        <v>User</v>
+      </c>
+      <c r="E47" t="str">
+        <v>/api/user</v>
+      </c>
+      <c r="F47" t="str">
+        <v>read</v>
+      </c>
+      <c r="G47" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H47" t="str">
+        <v>NEX  Admin  read all users (4) from 0 to 100</v>
+      </c>
+      <c r="I47">
+        <v>9</v>
+      </c>
+      <c r="J47" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K47" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L47" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B48" t="str">
+        <v>05:12:33 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D48" t="str">
+        <v>User</v>
+      </c>
+      <c r="E48" t="str">
+        <v>/api/user</v>
+      </c>
+      <c r="F48" t="str">
+        <v>read</v>
+      </c>
+      <c r="G48" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H48" t="str">
+        <v>NEX  Admin  read all users (4) from 0 to 100</v>
+      </c>
+      <c r="I48">
+        <v>9</v>
+      </c>
+      <c r="J48" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K48" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L48" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B49" t="str">
+        <v>05:12:34 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D49" t="str">
+        <v>Trip</v>
+      </c>
+      <c r="E49" t="str">
+        <v>/api/trip</v>
+      </c>
+      <c r="F49" t="str">
+        <v>read</v>
+      </c>
+      <c r="G49" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H49" t="str">
+        <v>NEX  Admin  read all trips (2) from 0 to 100</v>
+      </c>
+      <c r="I49">
+        <v>9</v>
+      </c>
+      <c r="J49" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K49" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L49" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B50" t="str">
+        <v>05:12:35 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D50" t="str">
+        <v>User</v>
+      </c>
+      <c r="E50" t="str">
+        <v>/api/user</v>
+      </c>
+      <c r="F50" t="str">
+        <v>read</v>
+      </c>
+      <c r="G50" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H50" t="str">
+        <v>NEX  Admin  read all users (4) from 0 to 100</v>
+      </c>
+      <c r="I50">
+        <v>9</v>
+      </c>
+      <c r="J50" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K50" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L50" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B51" t="str">
+        <v>05:12:36 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D51" t="str">
+        <v>User</v>
+      </c>
+      <c r="E51" t="str">
+        <v>/api/user</v>
+      </c>
+      <c r="F51" t="str">
+        <v>read</v>
+      </c>
+      <c r="G51" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H51" t="str">
+        <v>NEX  Admin  read all users (4) from 0 to 100</v>
+      </c>
+      <c r="I51">
+        <v>9</v>
+      </c>
+      <c r="J51" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K51" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L51" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B52" t="str">
+        <v>05:12:40 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D52" t="str">
+        <v>User</v>
+      </c>
+      <c r="E52" t="str">
+        <v>/api/user</v>
+      </c>
+      <c r="F52" t="str">
+        <v>read</v>
+      </c>
+      <c r="G52" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H52" t="str">
+        <v>NEX  Admin  read all users (4) from 0 to 100</v>
+      </c>
+      <c r="I52">
+        <v>9</v>
+      </c>
+      <c r="J52" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K52" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L52" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B53" t="str">
+        <v>05:12:40 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D53" t="str">
+        <v>User</v>
+      </c>
+      <c r="E53" t="str">
+        <v>/api/to-validate-users</v>
+      </c>
+      <c r="F53" t="str">
+        <v>read</v>
+      </c>
+      <c r="G53" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H53" t="str">
+        <v>NEX  Admin  read all to validate users (1) from 0 to 100</v>
+      </c>
+      <c r="I53">
+        <v>9</v>
+      </c>
+      <c r="J53" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K53" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L53" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B54" t="str">
+        <v>05:12:42 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D54" t="str">
+        <v>Trip</v>
+      </c>
+      <c r="E54" t="str">
+        <v>/api/trip</v>
+      </c>
+      <c r="F54" t="str">
+        <v>read</v>
+      </c>
+      <c r="G54" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H54" t="str">
+        <v>NEX  Admin  read all trips (2) from 0 to 100</v>
+      </c>
+      <c r="I54">
+        <v>9</v>
+      </c>
+      <c r="J54" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K54" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L54" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B55" t="str">
+        <v>05:15:08 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D55" t="str">
+        <v>Trip</v>
+      </c>
+      <c r="E55" t="str">
+        <v>/api/trip</v>
+      </c>
+      <c r="F55" t="str">
+        <v>read</v>
+      </c>
+      <c r="G55" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H55" t="str">
+        <v>NEX  Admin  read all trips (2) from 0 to 100</v>
+      </c>
+      <c r="I55">
+        <v>9</v>
+      </c>
+      <c r="J55" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K55" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L55" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B56" t="str">
+        <v>05:15:09 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D56" t="str">
+        <v>User</v>
+      </c>
+      <c r="E56" t="str">
+        <v>/api/to-validate-users</v>
+      </c>
+      <c r="F56" t="str">
+        <v>read</v>
+      </c>
+      <c r="G56" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H56" t="str">
+        <v>NEX  Admin  read all to validate users (1) from 0 to 100</v>
+      </c>
+      <c r="I56">
+        <v>9</v>
+      </c>
+      <c r="J56" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K56" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L56" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B57" t="str">
+        <v>05:15:13 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D57" t="str">
+        <v>Trip</v>
+      </c>
+      <c r="E57" t="str">
+        <v>/api/trip</v>
+      </c>
+      <c r="F57" t="str">
+        <v>read</v>
+      </c>
+      <c r="G57" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H57" t="str">
+        <v>NEX  Admin  read all trips (2) from 0 to 100</v>
+      </c>
+      <c r="I57">
+        <v>9</v>
+      </c>
+      <c r="J57" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K57" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L57" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B58" t="str">
+        <v>05:15:14 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D58" t="str">
+        <v>User</v>
+      </c>
+      <c r="E58" t="str">
+        <v>/api/to-validate-users</v>
+      </c>
+      <c r="F58" t="str">
+        <v>read</v>
+      </c>
+      <c r="G58" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H58" t="str">
+        <v>NEX  Admin  read all to validate users (1) from 0 to 100</v>
+      </c>
+      <c r="I58">
+        <v>9</v>
+      </c>
+      <c r="J58" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K58" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L58" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B59" t="str">
+        <v>05:15:15 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D59" t="str">
+        <v>User</v>
+      </c>
+      <c r="E59" t="str">
+        <v>/api/user</v>
+      </c>
+      <c r="F59" t="str">
+        <v>read</v>
+      </c>
+      <c r="G59" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H59" t="str">
+        <v>NEX  Admin  read all users (4) from 0 to 100</v>
+      </c>
+      <c r="I59">
+        <v>9</v>
+      </c>
+      <c r="J59" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K59" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L59" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B60" t="str">
+        <v>05:15:16 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D60" t="str">
+        <v>User</v>
+      </c>
+      <c r="E60" t="str">
+        <v>/api/to-validate-users</v>
+      </c>
+      <c r="F60" t="str">
+        <v>read</v>
+      </c>
+      <c r="G60" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H60" t="str">
+        <v>NEX  Admin  read all to validate users (1) from 0 to 100</v>
+      </c>
+      <c r="I60">
+        <v>9</v>
+      </c>
+      <c r="J60" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K60" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L60" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B61" t="str">
+        <v>05:15:20 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D61" t="str">
+        <v>Preference</v>
+      </c>
+      <c r="E61" t="str">
+        <v>/api/preference</v>
+      </c>
+      <c r="F61" t="str">
+        <v>read</v>
+      </c>
+      <c r="G61" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H61" t="str">
+        <v>NEX  Admin  read all preferences (undefined) from undefined to NaN</v>
+      </c>
+      <c r="I61">
+        <v>9</v>
+      </c>
+      <c r="J61" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K61" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L61" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B62" t="str">
+        <v>05:15:22 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D62" t="str">
+        <v>VehicleType</v>
+      </c>
+      <c r="E62" t="str">
+        <v>/api/vehicle-type</v>
+      </c>
+      <c r="F62" t="str">
+        <v>read</v>
+      </c>
+      <c r="G62" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H62" t="str">
+        <v>NEX  Admin  read all vehicle types (undefined) from undefined to NaN</v>
+      </c>
+      <c r="I62">
+        <v>9</v>
+      </c>
+      <c r="J62" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K62" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L62" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B63" t="str">
+        <v>05:15:25 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D63" t="str">
+        <v>Pricing</v>
+      </c>
+      <c r="E63" t="str">
+        <v>/api/pricing</v>
+      </c>
+      <c r="F63" t="str">
+        <v>read</v>
+      </c>
+      <c r="G63" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H63" t="str">
+        <v>NEX  Admin  read all pricing (undefined) from undefined to NaN</v>
+      </c>
+      <c r="I63">
+        <v>9</v>
+      </c>
+      <c r="J63" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K63" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L63" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B64" t="str">
+        <v>05:15:35 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D64" t="str">
+        <v>User</v>
+      </c>
+      <c r="E64" t="str">
+        <v>/api/user</v>
+      </c>
+      <c r="F64" t="str">
+        <v>read</v>
+      </c>
+      <c r="G64" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H64" t="str">
+        <v>NEX  Admin  read all users (4) from 0 to 100</v>
+      </c>
+      <c r="I64">
+        <v>9</v>
+      </c>
+      <c r="J64" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K64" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L64" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B65" t="str">
+        <v>05:15:38 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D65" t="str">
+        <v>Trip</v>
+      </c>
+      <c r="E65" t="str">
+        <v>/api/trip</v>
+      </c>
+      <c r="F65" t="str">
+        <v>read</v>
+      </c>
+      <c r="G65" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H65" t="str">
+        <v>NEX  Admin  read all trips (2) from 0 to 100</v>
+      </c>
+      <c r="I65">
+        <v>9</v>
+      </c>
+      <c r="J65" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K65" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L65" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B66" t="str">
+        <v>05:36:18 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D66" t="str">
+        <v>Trip</v>
+      </c>
+      <c r="E66" t="str">
+        <v>/api/trip</v>
+      </c>
+      <c r="F66" t="str">
+        <v>read</v>
+      </c>
+      <c r="G66" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H66" t="str">
+        <v>NEX  Admin  read all trips (2) from 0 to 100</v>
+      </c>
+      <c r="I66">
+        <v>9</v>
+      </c>
+      <c r="J66" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K66" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L66" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B67" t="str">
+        <v>05:36:24 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D67" t="str">
+        <v>Trip</v>
+      </c>
+      <c r="E67" t="str">
+        <v>/api/trip</v>
+      </c>
+      <c r="F67" t="str">
+        <v>read</v>
+      </c>
+      <c r="G67" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H67" t="str">
+        <v>NEX  Admin  read all trips (2) from 0 to 100</v>
+      </c>
+      <c r="I67">
+        <v>9</v>
+      </c>
+      <c r="J67" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K67" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L67" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B68" t="str">
+        <v>05:37:09 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D68" t="str">
+        <v>Trip</v>
+      </c>
+      <c r="E68" t="str">
+        <v>/api/trip</v>
+      </c>
+      <c r="F68" t="str">
+        <v>read</v>
+      </c>
+      <c r="G68" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H68" t="str">
+        <v>NEX  Admin  read all trips (2) from 0 to 100</v>
+      </c>
+      <c r="I68">
+        <v>9</v>
+      </c>
+      <c r="J68" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K68" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L68" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B69" t="str">
+        <v>05:37:12 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D69" t="str">
+        <v>User</v>
+      </c>
+      <c r="E69" t="str">
+        <v>/api/to-validate-users</v>
+      </c>
+      <c r="F69" t="str">
+        <v>read</v>
+      </c>
+      <c r="G69" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H69" t="str">
+        <v>NEX  Admin  read all to validate users (1) from 0 to 100</v>
+      </c>
+      <c r="I69">
+        <v>9</v>
+      </c>
+      <c r="J69" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K69" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L69" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B70" t="str">
+        <v>05:37:13 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D70" t="str">
+        <v>User</v>
+      </c>
+      <c r="E70" t="str">
+        <v>/api/user</v>
+      </c>
+      <c r="F70" t="str">
+        <v>read</v>
+      </c>
+      <c r="G70" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H70" t="str">
+        <v>NEX  Admin  read all users (4) from 0 to 100</v>
+      </c>
+      <c r="I70">
+        <v>9</v>
+      </c>
+      <c r="J70" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K70" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L70" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B71" t="str">
+        <v>05:37:13 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D71" t="str">
+        <v>User</v>
+      </c>
+      <c r="E71" t="str">
+        <v>/api/user</v>
+      </c>
+      <c r="F71" t="str">
+        <v>read</v>
+      </c>
+      <c r="G71" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H71" t="str">
+        <v>NEX  Admin  read all users (4) from 0 to 100</v>
+      </c>
+      <c r="I71">
+        <v>9</v>
+      </c>
+      <c r="J71" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K71" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L71" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>Fri Sep 02 2022</v>
+      </c>
+      <c r="B72" t="str">
+        <v>05:37:16 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D72" t="str">
+        <v>Trip</v>
+      </c>
+      <c r="E72" t="str">
+        <v>/api/trip</v>
+      </c>
+      <c r="F72" t="str">
+        <v>read</v>
+      </c>
+      <c r="G72" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H72" t="str">
+        <v>NEX  Admin  read all trips (2) from 0 to 100</v>
+      </c>
+      <c r="I72">
+        <v>9</v>
+      </c>
+      <c r="J72" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K72" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L72" t="str">
+        <v>all</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:L72"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Remove vehicle types constraint, random PIN, pricing
</commit_message>
<xml_diff>
--- a/user-logs/data.xlsx
+++ b/user-logs/data.xlsx
@@ -16059,7 +16059,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N287"/>
+  <dimension ref="A1:N336"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -26250,9 +26250,1706 @@
         <v>1</v>
       </c>
     </row>
+    <row r="288">
+      <c r="A288" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B288" t="str">
+        <v>09:32:23 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="C288" t="str">
+        <v>developer@nex-softwares.com</v>
+      </c>
+      <c r="D288" t="str">
+        <v>User</v>
+      </c>
+      <c r="E288" t="str">
+        <v>/api/auth/login</v>
+      </c>
+      <c r="F288" t="str">
+        <v>login</v>
+      </c>
+      <c r="G288" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H288" t="str">
+        <v>developer@nex-softwares.com  login</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B289" t="str">
+        <v>09:32:23 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D289" t="str">
+        <v>User</v>
+      </c>
+      <c r="E289" t="str">
+        <v>/api/user</v>
+      </c>
+      <c r="F289" t="str">
+        <v>read</v>
+      </c>
+      <c r="G289" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H289" t="str">
+        <v>NEX  Admin  read all users (3) from 0 to 100</v>
+      </c>
+      <c r="I289">
+        <v>1</v>
+      </c>
+      <c r="J289" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K289" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L289" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B290" t="str">
+        <v>09:32:29 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D290" t="str">
+        <v>User</v>
+      </c>
+      <c r="E290" t="str">
+        <v>/api/user</v>
+      </c>
+      <c r="F290" t="str">
+        <v>read</v>
+      </c>
+      <c r="G290" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H290" t="str">
+        <v>NEX  Admin  read all users (3) from 0 to 100</v>
+      </c>
+      <c r="I290">
+        <v>1</v>
+      </c>
+      <c r="J290" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K290" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L290" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B291" t="str">
+        <v>09:33:53 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D291" t="str">
+        <v>User</v>
+      </c>
+      <c r="E291" t="str">
+        <v>/api/user/:id</v>
+      </c>
+      <c r="F291" t="str">
+        <v>read</v>
+      </c>
+      <c r="G291" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H291" t="str">
+        <v>NEX  Admin  read user 2</v>
+      </c>
+      <c r="I291">
+        <v>1</v>
+      </c>
+      <c r="J291" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K291" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L291" t="str">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B292" t="str">
+        <v>09:35:47 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D292" t="str">
+        <v>User</v>
+      </c>
+      <c r="E292" t="str">
+        <v>/api/user</v>
+      </c>
+      <c r="F292" t="str">
+        <v>read</v>
+      </c>
+      <c r="G292" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H292" t="str">
+        <v>NEX  Admin  read all users (3) from 0 to 100</v>
+      </c>
+      <c r="I292">
+        <v>1</v>
+      </c>
+      <c r="J292" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K292" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L292" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B293" t="str">
+        <v>09:35:47 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D293" t="str">
+        <v>User</v>
+      </c>
+      <c r="E293" t="str">
+        <v>/api/to-validate-users</v>
+      </c>
+      <c r="F293" t="str">
+        <v>read</v>
+      </c>
+      <c r="G293" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H293" t="str">
+        <v>NEX  Admin  read all to validate users (0) from 0 to 100</v>
+      </c>
+      <c r="I293">
+        <v>1</v>
+      </c>
+      <c r="J293" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K293" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L293" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B294" t="str">
+        <v>09:35:53 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D294" t="str">
+        <v>Trip</v>
+      </c>
+      <c r="E294" t="str">
+        <v>/api/trip</v>
+      </c>
+      <c r="F294" t="str">
+        <v>read</v>
+      </c>
+      <c r="G294" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H294" t="str">
+        <v>NEX  Admin  read all trips (1) from 0 to 100</v>
+      </c>
+      <c r="I294">
+        <v>1</v>
+      </c>
+      <c r="J294" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K294" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L294" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B295" t="str">
+        <v>09:37:25 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D295" t="str">
+        <v>User</v>
+      </c>
+      <c r="E295" t="str">
+        <v>/api/user</v>
+      </c>
+      <c r="F295" t="str">
+        <v>read</v>
+      </c>
+      <c r="G295" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H295" t="str">
+        <v>NEX  Admin  read all users (3) from 0 to 100</v>
+      </c>
+      <c r="I295">
+        <v>1</v>
+      </c>
+      <c r="J295" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K295" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L295" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B296" t="str">
+        <v>09:37:26 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D296" t="str">
+        <v>User</v>
+      </c>
+      <c r="E296" t="str">
+        <v>/api/user</v>
+      </c>
+      <c r="F296" t="str">
+        <v>read</v>
+      </c>
+      <c r="G296" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H296" t="str">
+        <v>NEX  Admin  read all users (3) from 0 to 100</v>
+      </c>
+      <c r="I296">
+        <v>1</v>
+      </c>
+      <c r="J296" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K296" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L296" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B297" t="str">
+        <v>09:37:27 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D297" t="str">
+        <v>User</v>
+      </c>
+      <c r="E297" t="str">
+        <v>/api/to-validate-users</v>
+      </c>
+      <c r="F297" t="str">
+        <v>read</v>
+      </c>
+      <c r="G297" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H297" t="str">
+        <v>NEX  Admin  read all to validate users (0) from 0 to 100</v>
+      </c>
+      <c r="I297">
+        <v>1</v>
+      </c>
+      <c r="J297" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K297" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L297" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B298" t="str">
+        <v>09:37:28 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D298" t="str">
+        <v>Trip</v>
+      </c>
+      <c r="E298" t="str">
+        <v>/api/trip</v>
+      </c>
+      <c r="F298" t="str">
+        <v>read</v>
+      </c>
+      <c r="G298" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H298" t="str">
+        <v>NEX  Admin  read all trips (1) from 0 to 100</v>
+      </c>
+      <c r="I298">
+        <v>1</v>
+      </c>
+      <c r="J298" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K298" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L298" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B299" t="str">
+        <v>09:37:48 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D299" t="str">
+        <v>User</v>
+      </c>
+      <c r="E299" t="str">
+        <v>/api/user</v>
+      </c>
+      <c r="F299" t="str">
+        <v>read</v>
+      </c>
+      <c r="G299" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H299" t="str">
+        <v>NEX  Admin  read all users (3) from 0 to 100</v>
+      </c>
+      <c r="I299">
+        <v>1</v>
+      </c>
+      <c r="J299" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K299" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L299" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B300" t="str">
+        <v>09:37:50 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D300" t="str">
+        <v>User</v>
+      </c>
+      <c r="E300" t="str">
+        <v>/api/user</v>
+      </c>
+      <c r="F300" t="str">
+        <v>read</v>
+      </c>
+      <c r="G300" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H300" t="str">
+        <v>NEX  Admin  read all users (3) from 0 to 100</v>
+      </c>
+      <c r="I300">
+        <v>1</v>
+      </c>
+      <c r="J300" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K300" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L300" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B301" t="str">
+        <v>09:37:52 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D301" t="str">
+        <v>User</v>
+      </c>
+      <c r="E301" t="str">
+        <v>/api/to-validate-users</v>
+      </c>
+      <c r="F301" t="str">
+        <v>read</v>
+      </c>
+      <c r="G301" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H301" t="str">
+        <v>NEX  Admin  read all to validate users (0) from 0 to 100</v>
+      </c>
+      <c r="I301">
+        <v>1</v>
+      </c>
+      <c r="J301" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K301" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L301" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B302" t="str">
+        <v>09:37:52 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D302" t="str">
+        <v>Trip</v>
+      </c>
+      <c r="E302" t="str">
+        <v>/api/trip</v>
+      </c>
+      <c r="F302" t="str">
+        <v>read</v>
+      </c>
+      <c r="G302" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H302" t="str">
+        <v>NEX  Admin  read all trips (1) from 0 to 100</v>
+      </c>
+      <c r="I302">
+        <v>1</v>
+      </c>
+      <c r="J302" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K302" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L302" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B303" t="str">
+        <v>09:38:10 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D303" t="str">
+        <v>Preference</v>
+      </c>
+      <c r="E303" t="str">
+        <v>/api/preference</v>
+      </c>
+      <c r="F303" t="str">
+        <v>read</v>
+      </c>
+      <c r="G303" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H303" t="str">
+        <v>NEX  Admin  read all preferences (undefined) from undefined to NaN</v>
+      </c>
+      <c r="I303">
+        <v>1</v>
+      </c>
+      <c r="J303" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K303" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L303" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B304" t="str">
+        <v>09:39:17 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D304" t="str">
+        <v>Preference</v>
+      </c>
+      <c r="E304" t="str">
+        <v>/api/preference</v>
+      </c>
+      <c r="F304" t="str">
+        <v>write</v>
+      </c>
+      <c r="G304" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H304" t="str">
+        <v>NEX  Admin  write preference 2</v>
+      </c>
+      <c r="I304">
+        <v>1</v>
+      </c>
+      <c r="J304" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K304" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L304">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B305" t="str">
+        <v>09:39:18 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D305" t="str">
+        <v>Preference</v>
+      </c>
+      <c r="E305" t="str">
+        <v>/api/preference</v>
+      </c>
+      <c r="F305" t="str">
+        <v>read</v>
+      </c>
+      <c r="G305" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H305" t="str">
+        <v>NEX  Admin  read all preferences (undefined) from undefined to NaN</v>
+      </c>
+      <c r="I305">
+        <v>1</v>
+      </c>
+      <c r="J305" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K305" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L305" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B306" t="str">
+        <v>09:42:04 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D306" t="str">
+        <v>Pricing</v>
+      </c>
+      <c r="E306" t="str">
+        <v>/api/pricing</v>
+      </c>
+      <c r="F306" t="str">
+        <v>read</v>
+      </c>
+      <c r="G306" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H306" t="str">
+        <v>NEX  Admin  read all pricing (undefined) from undefined to NaN</v>
+      </c>
+      <c r="I306">
+        <v>1</v>
+      </c>
+      <c r="J306" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K306" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L306" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B307" t="str">
+        <v>09:42:18 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D307" t="str">
+        <v>VehicleType</v>
+      </c>
+      <c r="E307" t="str">
+        <v>/api/vehicle-type</v>
+      </c>
+      <c r="F307" t="str">
+        <v>read</v>
+      </c>
+      <c r="G307" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H307" t="str">
+        <v>NEX  Admin  read all vehicle types (undefined) from undefined to NaN</v>
+      </c>
+      <c r="I307">
+        <v>1</v>
+      </c>
+      <c r="J307" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K307" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L307" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B308" t="str">
+        <v>09:44:17 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D308" t="str">
+        <v>Pricing</v>
+      </c>
+      <c r="E308" t="str">
+        <v>/api/pricing</v>
+      </c>
+      <c r="F308" t="str">
+        <v>read</v>
+      </c>
+      <c r="G308" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H308" t="str">
+        <v>NEX  Admin  read all pricing (undefined) from undefined to NaN</v>
+      </c>
+      <c r="I308">
+        <v>1</v>
+      </c>
+      <c r="J308" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K308" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L308" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B309" t="str">
+        <v>09:46:45 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D309" t="str">
+        <v>User</v>
+      </c>
+      <c r="E309" t="str">
+        <v>/api/to-validate-users</v>
+      </c>
+      <c r="F309" t="str">
+        <v>read</v>
+      </c>
+      <c r="G309" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H309" t="str">
+        <v>NEX  Admin  read all to validate users (0) from 0 to 100</v>
+      </c>
+      <c r="I309">
+        <v>1</v>
+      </c>
+      <c r="J309" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K309" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L309" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B310" t="str">
+        <v>09:48:53 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D310" t="str">
+        <v>User</v>
+      </c>
+      <c r="E310" t="str">
+        <v>/api/auth/upload-document</v>
+      </c>
+      <c r="F310" t="str">
+        <v>upload</v>
+      </c>
+      <c r="G310" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H310" t="str">
+        <v>John  DOE  upload his documents</v>
+      </c>
+      <c r="I310">
+        <v>2</v>
+      </c>
+      <c r="J310" t="str">
+        <v>John</v>
+      </c>
+      <c r="K310" t="str">
+        <v>DOE</v>
+      </c>
+      <c r="L310" t="str">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B311" t="str">
+        <v>09:49:02 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D311" t="str">
+        <v>User</v>
+      </c>
+      <c r="E311" t="str">
+        <v>/api/to-validate-users</v>
+      </c>
+      <c r="F311" t="str">
+        <v>read</v>
+      </c>
+      <c r="G311" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H311" t="str">
+        <v>NEX  Admin  read all to validate users (1) from 0 to 100</v>
+      </c>
+      <c r="I311">
+        <v>1</v>
+      </c>
+      <c r="J311" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K311" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L311" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B312" t="str">
+        <v>10:06:23 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D312" t="str">
+        <v>User</v>
+      </c>
+      <c r="E312" t="str">
+        <v>/api/user</v>
+      </c>
+      <c r="F312" t="str">
+        <v>read</v>
+      </c>
+      <c r="G312" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H312" t="str">
+        <v>NEX  Admin  read all users (3) from 0 to 100</v>
+      </c>
+      <c r="I312">
+        <v>1</v>
+      </c>
+      <c r="J312" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K312" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L312" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B313" t="str">
+        <v>10:06:57 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D313" t="str">
+        <v>User</v>
+      </c>
+      <c r="E313" t="str">
+        <v>/api/to-validate-users</v>
+      </c>
+      <c r="F313" t="str">
+        <v>read</v>
+      </c>
+      <c r="G313" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H313" t="str">
+        <v>NEX  Admin  read all to validate users (1) from 0 to 100</v>
+      </c>
+      <c r="I313">
+        <v>1</v>
+      </c>
+      <c r="J313" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K313" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L313" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B314" t="str">
+        <v>10:06:58 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D314" t="str">
+        <v>Trip</v>
+      </c>
+      <c r="E314" t="str">
+        <v>/api/trip</v>
+      </c>
+      <c r="F314" t="str">
+        <v>read</v>
+      </c>
+      <c r="G314" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H314" t="str">
+        <v>NEX  Admin  read all trips (1) from 0 to 100</v>
+      </c>
+      <c r="I314">
+        <v>1</v>
+      </c>
+      <c r="J314" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K314" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L314" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B315" t="str">
+        <v>10:07:02 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D315" t="str">
+        <v>Preference</v>
+      </c>
+      <c r="E315" t="str">
+        <v>/api/preference</v>
+      </c>
+      <c r="F315" t="str">
+        <v>read</v>
+      </c>
+      <c r="G315" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H315" t="str">
+        <v>NEX  Admin  read all preferences (undefined) from undefined to NaN</v>
+      </c>
+      <c r="I315">
+        <v>1</v>
+      </c>
+      <c r="J315" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K315" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L315" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B316" t="str">
+        <v>10:07:06 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D316" t="str">
+        <v>VehicleType</v>
+      </c>
+      <c r="E316" t="str">
+        <v>/api/vehicle-type</v>
+      </c>
+      <c r="F316" t="str">
+        <v>read</v>
+      </c>
+      <c r="G316" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H316" t="str">
+        <v>NEX  Admin  read all vehicle types (undefined) from undefined to NaN</v>
+      </c>
+      <c r="I316">
+        <v>1</v>
+      </c>
+      <c r="J316" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K316" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L316" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B317" t="str">
+        <v>10:07:08 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D317" t="str">
+        <v>Pricing</v>
+      </c>
+      <c r="E317" t="str">
+        <v>/api/pricing</v>
+      </c>
+      <c r="F317" t="str">
+        <v>read</v>
+      </c>
+      <c r="G317" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H317" t="str">
+        <v>NEX  Admin  read all pricing (undefined) from undefined to NaN</v>
+      </c>
+      <c r="I317">
+        <v>1</v>
+      </c>
+      <c r="J317" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K317" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L317" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B318" t="str">
+        <v>10:07:17 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D318" t="str">
+        <v>User</v>
+      </c>
+      <c r="E318" t="str">
+        <v>/api/user</v>
+      </c>
+      <c r="F318" t="str">
+        <v>read</v>
+      </c>
+      <c r="G318" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H318" t="str">
+        <v>NEX  Admin  read all users (3) from 0 to 100</v>
+      </c>
+      <c r="I318">
+        <v>1</v>
+      </c>
+      <c r="J318" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K318" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L318" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B319" t="str">
+        <v>10:11:03 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D319" t="str">
+        <v>User</v>
+      </c>
+      <c r="E319" t="str">
+        <v>/api/auth/logout</v>
+      </c>
+      <c r="F319" t="str">
+        <v>logout</v>
+      </c>
+      <c r="G319" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H319" t="str">
+        <v xml:space="preserve">NEX  Admin  logout </v>
+      </c>
+      <c r="I319">
+        <v>1</v>
+      </c>
+      <c r="J319" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K319" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L319" t="str">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B320" t="str">
+        <v>13:24:35 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="C320" t="str">
+        <v>developer@nex-softwares.com</v>
+      </c>
+      <c r="D320" t="str">
+        <v>User</v>
+      </c>
+      <c r="E320" t="str">
+        <v>/api/auth/login</v>
+      </c>
+      <c r="F320" t="str">
+        <v>login</v>
+      </c>
+      <c r="G320" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H320" t="str">
+        <v>developer@nex-softwares.com  login</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B321" t="str">
+        <v>13:24:36 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D321" t="str">
+        <v>User</v>
+      </c>
+      <c r="E321" t="str">
+        <v>/api/user</v>
+      </c>
+      <c r="F321" t="str">
+        <v>read</v>
+      </c>
+      <c r="G321" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H321" t="str">
+        <v>NEX  Admin  read all users (3) from 0 to 100</v>
+      </c>
+      <c r="I321">
+        <v>1</v>
+      </c>
+      <c r="J321" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K321" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L321" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B322" t="str">
+        <v>13:24:39 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D322" t="str">
+        <v>User</v>
+      </c>
+      <c r="E322" t="str">
+        <v>/api/user</v>
+      </c>
+      <c r="F322" t="str">
+        <v>read</v>
+      </c>
+      <c r="G322" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H322" t="str">
+        <v>NEX  Admin  read all users (3) from 0 to 100</v>
+      </c>
+      <c r="I322">
+        <v>1</v>
+      </c>
+      <c r="J322" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K322" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L322" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B323" t="str">
+        <v>13:24:52 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D323" t="str">
+        <v>User</v>
+      </c>
+      <c r="E323" t="str">
+        <v>/api/to-validate-users</v>
+      </c>
+      <c r="F323" t="str">
+        <v>read</v>
+      </c>
+      <c r="G323" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H323" t="str">
+        <v>NEX  Admin  read all to validate users (1) from 0 to 100</v>
+      </c>
+      <c r="I323">
+        <v>1</v>
+      </c>
+      <c r="J323" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K323" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L323" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B324" t="str">
+        <v>13:25:25 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D324" t="str">
+        <v>User</v>
+      </c>
+      <c r="E324" t="str">
+        <v>/api/to-validate-users</v>
+      </c>
+      <c r="F324" t="str">
+        <v>read</v>
+      </c>
+      <c r="G324" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H324" t="str">
+        <v>NEX  Admin  read all to validate users (1) from 0 to 100</v>
+      </c>
+      <c r="I324">
+        <v>1</v>
+      </c>
+      <c r="J324" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K324" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L324" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B325" t="str">
+        <v>13:25:56 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D325" t="str">
+        <v>Trip</v>
+      </c>
+      <c r="E325" t="str">
+        <v>/api/trip</v>
+      </c>
+      <c r="F325" t="str">
+        <v>read</v>
+      </c>
+      <c r="G325" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H325" t="str">
+        <v>NEX  Admin  read all trips (1) from 0 to 100</v>
+      </c>
+      <c r="I325">
+        <v>1</v>
+      </c>
+      <c r="J325" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K325" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L325" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B326" t="str">
+        <v>13:26:19 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D326" t="str">
+        <v>User</v>
+      </c>
+      <c r="E326" t="str">
+        <v>/api/user</v>
+      </c>
+      <c r="F326" t="str">
+        <v>read</v>
+      </c>
+      <c r="G326" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H326" t="str">
+        <v>NEX  Admin  read all users (3) from 0 to 100</v>
+      </c>
+      <c r="I326">
+        <v>1</v>
+      </c>
+      <c r="J326" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K326" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L326" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B327" t="str">
+        <v>13:26:21 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D327" t="str">
+        <v>User</v>
+      </c>
+      <c r="E327" t="str">
+        <v>/api/user/:id</v>
+      </c>
+      <c r="F327" t="str">
+        <v>read</v>
+      </c>
+      <c r="G327" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H327" t="str">
+        <v>NEX  Admin  read user 2</v>
+      </c>
+      <c r="I327">
+        <v>1</v>
+      </c>
+      <c r="J327" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K327" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L327" t="str">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B328" t="str">
+        <v>13:27:08 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D328" t="str">
+        <v>Trip</v>
+      </c>
+      <c r="E328" t="str">
+        <v>/api/trip</v>
+      </c>
+      <c r="F328" t="str">
+        <v>read</v>
+      </c>
+      <c r="G328" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H328" t="str">
+        <v>NEX  Admin  read all trips (1) from 0 to 100</v>
+      </c>
+      <c r="I328">
+        <v>1</v>
+      </c>
+      <c r="J328" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K328" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L328" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B329" t="str">
+        <v>13:27:24 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D329" t="str">
+        <v>Preference</v>
+      </c>
+      <c r="E329" t="str">
+        <v>/api/preference</v>
+      </c>
+      <c r="F329" t="str">
+        <v>read</v>
+      </c>
+      <c r="G329" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H329" t="str">
+        <v>NEX  Admin  read all preferences (undefined) from undefined to NaN</v>
+      </c>
+      <c r="I329">
+        <v>1</v>
+      </c>
+      <c r="J329" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K329" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L329" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B330" t="str">
+        <v>13:27:40 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D330" t="str">
+        <v>VehicleType</v>
+      </c>
+      <c r="E330" t="str">
+        <v>/api/vehicle-type</v>
+      </c>
+      <c r="F330" t="str">
+        <v>read</v>
+      </c>
+      <c r="G330" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H330" t="str">
+        <v>NEX  Admin  read all vehicle types (undefined) from undefined to NaN</v>
+      </c>
+      <c r="I330">
+        <v>1</v>
+      </c>
+      <c r="J330" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K330" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L330" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B331" t="str">
+        <v>13:28:00 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D331" t="str">
+        <v>Pricing</v>
+      </c>
+      <c r="E331" t="str">
+        <v>/api/pricing</v>
+      </c>
+      <c r="F331" t="str">
+        <v>read</v>
+      </c>
+      <c r="G331" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H331" t="str">
+        <v>NEX  Admin  read all pricing (undefined) from undefined to NaN</v>
+      </c>
+      <c r="I331">
+        <v>1</v>
+      </c>
+      <c r="J331" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K331" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L331" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B332" t="str">
+        <v>13:28:26 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D332" t="str">
+        <v>Pricing</v>
+      </c>
+      <c r="E332" t="str">
+        <v>/api/pricing</v>
+      </c>
+      <c r="F332" t="str">
+        <v>write</v>
+      </c>
+      <c r="G332" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H332" t="str">
+        <v>NEX  Admin  write pricing 8</v>
+      </c>
+      <c r="I332">
+        <v>1</v>
+      </c>
+      <c r="J332" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K332" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L332">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B333" t="str">
+        <v>13:28:26 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D333" t="str">
+        <v>Pricing</v>
+      </c>
+      <c r="E333" t="str">
+        <v>/api/pricing</v>
+      </c>
+      <c r="F333" t="str">
+        <v>read</v>
+      </c>
+      <c r="G333" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H333" t="str">
+        <v>NEX  Admin  read all pricing (undefined) from undefined to NaN</v>
+      </c>
+      <c r="I333">
+        <v>1</v>
+      </c>
+      <c r="J333" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K333" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L333" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B334" t="str">
+        <v>13:28:44 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D334" t="str">
+        <v>Pricing</v>
+      </c>
+      <c r="E334" t="str">
+        <v>/api/pricing</v>
+      </c>
+      <c r="F334" t="str">
+        <v>edit</v>
+      </c>
+      <c r="G334" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H334" t="str">
+        <v>NEX  Admin  edit pricing 8</v>
+      </c>
+      <c r="I334">
+        <v>1</v>
+      </c>
+      <c r="J334" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K334" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L334">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B335" t="str">
+        <v>13:28:44 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D335" t="str">
+        <v>Pricing</v>
+      </c>
+      <c r="E335" t="str">
+        <v>/api/pricing</v>
+      </c>
+      <c r="F335" t="str">
+        <v>read</v>
+      </c>
+      <c r="G335" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H335" t="str">
+        <v>NEX  Admin  read all pricing (undefined) from undefined to NaN</v>
+      </c>
+      <c r="I335">
+        <v>1</v>
+      </c>
+      <c r="J335" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K335" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L335" t="str">
+        <v>all</v>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="str">
+        <v>Sun Sep 04 2022</v>
+      </c>
+      <c r="B336" t="str">
+        <v>13:28:51 GMT+0000 (Coordinated Universal Time)</v>
+      </c>
+      <c r="D336" t="str">
+        <v>Pricing</v>
+      </c>
+      <c r="E336" t="str">
+        <v>/api/pricing</v>
+      </c>
+      <c r="F336" t="str">
+        <v>read</v>
+      </c>
+      <c r="G336" t="str">
+        <v>succeeded</v>
+      </c>
+      <c r="H336" t="str">
+        <v>NEX  Admin  read all pricing (undefined) from undefined to NaN</v>
+      </c>
+      <c r="I336">
+        <v>1</v>
+      </c>
+      <c r="J336" t="str">
+        <v>NEX</v>
+      </c>
+      <c r="K336" t="str">
+        <v>Admin</v>
+      </c>
+      <c r="L336" t="str">
+        <v>all</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N287"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N336"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>